<commit_message>
Added tax locations to properties
</commit_message>
<xml_diff>
--- a/resources/info.xlsx
+++ b/resources/info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\moi\programming things\0.projects\monopoly-discord-bot\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C272258B-7BB9-4FB5-B815-85286A964A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B231AFAB-08AD-4DC9-A9FB-83F2EB44A2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
   <si>
     <t>PropertyUS</t>
   </si>
@@ -230,13 +230,19 @@
   </si>
   <si>
     <t>Get out of jail free</t>
+  </si>
+  <si>
+    <t>Income Tax</t>
+  </si>
+  <si>
+    <t>Super Tax</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,11 +382,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="42">
@@ -778,7 +779,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -789,11 +790,12 @@
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1158,56 +1160,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="11.54296875" customWidth="1"/>
+    <col min="1" max="2" width="11.54296875" style="10" customWidth="1"/>
+    <col min="3" max="13" width="6.08984375" style="10"/>
     <col min="14" max="14" width="6.08984375" style="9"/>
+    <col min="15" max="16384" width="6.08984375" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="10" t="s">
         <v>8</v>
       </c>
       <c r="N1" s="9" t="s">
@@ -1221,40 +1225,40 @@
       <c r="B2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="10">
         <v>60</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="10">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="10">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="10">
         <v>10</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="10">
         <v>30</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="10">
         <v>90</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="10">
         <v>160</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="10">
         <v>250</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="10">
         <v>50</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="10">
         <v>30</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="10">
         <v>33</v>
       </c>
-      <c r="N2" s="10">
+      <c r="N2" s="13">
         <v>1</v>
       </c>
     </row>
@@ -1265,37 +1269,37 @@
       <c r="B3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="10">
         <v>60</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="10">
         <v>4</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="10">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="10">
         <v>20</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="10">
         <v>60</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="10">
         <v>180</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="10">
         <v>320</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="10">
         <v>450</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="10">
         <v>50</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="10">
         <v>30</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="10">
         <v>33</v>
       </c>
       <c r="N3" s="9">
@@ -1303,1080 +1307,1111 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="10">
+        <v>200</v>
+      </c>
+      <c r="N4" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C4">
+      <c r="C5" s="10">
         <v>200</v>
       </c>
-      <c r="F4">
+      <c r="F5" s="10">
         <v>25</v>
       </c>
-      <c r="G4">
+      <c r="G5" s="10">
         <v>50</v>
       </c>
-      <c r="H4">
+      <c r="H5" s="10">
         <v>100</v>
       </c>
-      <c r="I4">
+      <c r="I5" s="10">
         <v>200</v>
       </c>
-      <c r="L4">
+      <c r="L5" s="10">
         <v>100</v>
       </c>
-      <c r="M4">
+      <c r="M5" s="10">
         <v>110</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N5" s="9">
         <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5">
-        <v>100</v>
-      </c>
-      <c r="D5">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>30</v>
-      </c>
-      <c r="G5">
-        <v>90</v>
-      </c>
-      <c r="H5">
-        <v>270</v>
-      </c>
-      <c r="I5">
-        <v>400</v>
-      </c>
-      <c r="J5">
-        <v>550</v>
-      </c>
-      <c r="K5">
-        <v>50</v>
-      </c>
-      <c r="L5">
-        <v>50</v>
-      </c>
-      <c r="M5">
-        <v>55</v>
-      </c>
-      <c r="N5" s="9">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6">
+        <v>16</v>
+      </c>
+      <c r="C6" s="10">
         <v>100</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="10">
         <v>6</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="10">
         <v>1</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="10">
         <v>30</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="10">
         <v>90</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="10">
         <v>270</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="10">
         <v>400</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="10">
         <v>550</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="10">
         <v>50</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="10">
         <v>50</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="10">
         <v>55</v>
       </c>
       <c r="N6" s="9">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="10">
+        <v>100</v>
+      </c>
+      <c r="D7" s="10">
+        <v>6</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10">
+        <v>30</v>
+      </c>
+      <c r="G7" s="10">
+        <v>90</v>
+      </c>
+      <c r="H7" s="10">
+        <v>270</v>
+      </c>
+      <c r="I7" s="10">
+        <v>400</v>
+      </c>
+      <c r="J7" s="10">
+        <v>550</v>
+      </c>
+      <c r="K7" s="10">
+        <v>50</v>
+      </c>
+      <c r="L7" s="10">
+        <v>50</v>
+      </c>
+      <c r="M7" s="10">
+        <v>55</v>
+      </c>
+      <c r="N7" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C7">
+      <c r="C8" s="10">
         <v>120</v>
       </c>
-      <c r="D7">
+      <c r="D8" s="10">
         <v>8</v>
       </c>
-      <c r="E7">
+      <c r="E8" s="10">
         <v>1</v>
       </c>
-      <c r="F7">
+      <c r="F8" s="10">
         <v>40</v>
       </c>
-      <c r="G7">
+      <c r="G8" s="10">
         <v>100</v>
       </c>
-      <c r="H7">
+      <c r="H8" s="10">
         <v>300</v>
       </c>
-      <c r="I7">
+      <c r="I8" s="10">
         <v>450</v>
       </c>
-      <c r="J7">
+      <c r="J8" s="10">
         <v>600</v>
       </c>
-      <c r="K7">
+      <c r="K8" s="10">
         <v>50</v>
       </c>
-      <c r="L7">
+      <c r="L8" s="10">
         <v>60</v>
       </c>
-      <c r="M7">
+      <c r="M8" s="10">
         <v>66</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N8" s="9">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C8">
+      <c r="C9" s="10">
         <v>140</v>
       </c>
-      <c r="D8">
+      <c r="D9" s="10">
         <v>10</v>
       </c>
-      <c r="E8">
+      <c r="E9" s="10">
         <v>2</v>
       </c>
-      <c r="F8">
+      <c r="F9" s="10">
         <v>50</v>
       </c>
-      <c r="G8">
+      <c r="G9" s="10">
         <v>150</v>
       </c>
-      <c r="H8">
+      <c r="H9" s="10">
         <v>450</v>
       </c>
-      <c r="I8">
+      <c r="I9" s="10">
         <v>625</v>
       </c>
-      <c r="J8">
+      <c r="J9" s="10">
         <v>750</v>
       </c>
-      <c r="K8">
+      <c r="K9" s="10">
         <v>100</v>
       </c>
-      <c r="L8">
+      <c r="L9" s="10">
         <v>70</v>
       </c>
-      <c r="M8">
+      <c r="M9" s="10">
         <v>77</v>
       </c>
-      <c r="N8" s="9">
+      <c r="N9" s="9">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C9">
+      <c r="C10" s="10">
         <v>150</v>
       </c>
-      <c r="F9">
+      <c r="F10" s="10">
         <v>4</v>
       </c>
-      <c r="G9">
+      <c r="G10" s="10">
         <v>10</v>
       </c>
-      <c r="L9">
+      <c r="L10" s="10">
         <v>75</v>
       </c>
-      <c r="M9">
+      <c r="M10" s="10">
         <v>83</v>
       </c>
-      <c r="N9" s="9">
+      <c r="N10" s="9">
         <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10">
-        <v>140</v>
-      </c>
-      <c r="D10">
-        <v>10</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="F10">
-        <v>50</v>
-      </c>
-      <c r="G10">
-        <v>150</v>
-      </c>
-      <c r="H10">
-        <v>450</v>
-      </c>
-      <c r="I10">
-        <v>625</v>
-      </c>
-      <c r="J10">
-        <v>750</v>
-      </c>
-      <c r="K10">
-        <v>100</v>
-      </c>
-      <c r="L10">
-        <v>70</v>
-      </c>
-      <c r="M10">
-        <v>77</v>
-      </c>
-      <c r="N10" s="9">
-        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="10">
+        <v>140</v>
+      </c>
+      <c r="D11" s="10">
+        <v>10</v>
+      </c>
+      <c r="E11" s="10">
+        <v>2</v>
+      </c>
+      <c r="F11" s="10">
+        <v>50</v>
+      </c>
+      <c r="G11" s="10">
+        <v>150</v>
+      </c>
+      <c r="H11" s="10">
+        <v>450</v>
+      </c>
+      <c r="I11" s="10">
+        <v>625</v>
+      </c>
+      <c r="J11" s="10">
+        <v>750</v>
+      </c>
+      <c r="K11" s="10">
+        <v>100</v>
+      </c>
+      <c r="L11" s="10">
+        <v>70</v>
+      </c>
+      <c r="M11" s="10">
+        <v>77</v>
+      </c>
+      <c r="N11" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C11">
+      <c r="C12" s="10">
         <v>160</v>
       </c>
-      <c r="D11">
+      <c r="D12" s="10">
         <v>12</v>
       </c>
-      <c r="E11">
+      <c r="E12" s="10">
         <v>2</v>
       </c>
-      <c r="F11">
+      <c r="F12" s="10">
         <v>60</v>
       </c>
-      <c r="G11">
+      <c r="G12" s="10">
         <v>180</v>
       </c>
-      <c r="H11">
+      <c r="H12" s="10">
         <v>500</v>
       </c>
-      <c r="I11">
+      <c r="I12" s="10">
         <v>700</v>
       </c>
-      <c r="J11">
+      <c r="J12" s="10">
         <v>900</v>
       </c>
-      <c r="K11">
+      <c r="K12" s="10">
         <v>100</v>
       </c>
-      <c r="L11">
+      <c r="L12" s="10">
         <v>80</v>
       </c>
-      <c r="M11">
+      <c r="M12" s="10">
         <v>88</v>
       </c>
-      <c r="N11" s="9">
+      <c r="N12" s="9">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C12">
+      <c r="C13" s="10">
         <v>200</v>
       </c>
-      <c r="F12">
+      <c r="F13" s="10">
         <v>25</v>
       </c>
-      <c r="G12">
+      <c r="G13" s="10">
         <v>50</v>
       </c>
-      <c r="H12">
+      <c r="H13" s="10">
         <v>100</v>
       </c>
-      <c r="I12">
+      <c r="I13" s="10">
         <v>200</v>
       </c>
-      <c r="L12">
+      <c r="L13" s="10">
         <v>100</v>
       </c>
-      <c r="M12">
+      <c r="M13" s="10">
         <v>110</v>
       </c>
-      <c r="N12" s="9">
+      <c r="N13" s="9">
         <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13">
-        <v>180</v>
-      </c>
-      <c r="D13">
-        <v>14</v>
-      </c>
-      <c r="E13">
-        <v>3</v>
-      </c>
-      <c r="F13">
-        <v>70</v>
-      </c>
-      <c r="G13">
-        <v>200</v>
-      </c>
-      <c r="H13">
-        <v>550</v>
-      </c>
-      <c r="I13">
-        <v>750</v>
-      </c>
-      <c r="J13">
-        <v>950</v>
-      </c>
-      <c r="K13">
-        <v>100</v>
-      </c>
-      <c r="L13">
-        <v>90</v>
-      </c>
-      <c r="M13">
-        <v>99</v>
-      </c>
-      <c r="N13" s="9">
-        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14">
+        <v>31</v>
+      </c>
+      <c r="C14" s="10">
         <v>180</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="10">
         <v>14</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="10">
         <v>3</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="10">
         <v>70</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="10">
         <v>200</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="10">
         <v>550</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="10">
         <v>750</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="10">
         <v>950</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="10">
         <v>100</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="10">
         <v>90</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="10">
         <v>99</v>
       </c>
       <c r="N14" s="9">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="10">
+        <v>180</v>
+      </c>
+      <c r="D15" s="10">
+        <v>14</v>
+      </c>
+      <c r="E15" s="10">
+        <v>3</v>
+      </c>
+      <c r="F15" s="10">
+        <v>70</v>
+      </c>
+      <c r="G15" s="10">
+        <v>200</v>
+      </c>
+      <c r="H15" s="10">
+        <v>550</v>
+      </c>
+      <c r="I15" s="10">
+        <v>750</v>
+      </c>
+      <c r="J15" s="10">
+        <v>950</v>
+      </c>
+      <c r="K15" s="10">
+        <v>100</v>
+      </c>
+      <c r="L15" s="10">
+        <v>90</v>
+      </c>
+      <c r="M15" s="10">
+        <v>99</v>
+      </c>
+      <c r="N15" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C15">
+      <c r="C16" s="10">
         <v>200</v>
       </c>
-      <c r="D15">
+      <c r="D16" s="10">
         <v>16</v>
       </c>
-      <c r="E15">
+      <c r="E16" s="10">
         <v>3</v>
       </c>
-      <c r="F15">
+      <c r="F16" s="10">
         <v>80</v>
       </c>
-      <c r="G15">
+      <c r="G16" s="10">
         <v>220</v>
       </c>
-      <c r="H15">
+      <c r="H16" s="10">
         <v>600</v>
       </c>
-      <c r="I15">
+      <c r="I16" s="10">
         <v>800</v>
       </c>
-      <c r="J15">
+      <c r="J16" s="10">
         <v>1000</v>
       </c>
-      <c r="K15">
+      <c r="K16" s="10">
         <v>100</v>
       </c>
-      <c r="L15">
+      <c r="L16" s="10">
         <v>100</v>
       </c>
-      <c r="M15">
+      <c r="M16" s="10">
         <v>110</v>
       </c>
-      <c r="N15" s="9">
+      <c r="N16" s="9">
         <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16">
-        <v>220</v>
-      </c>
-      <c r="D16">
-        <v>18</v>
-      </c>
-      <c r="E16">
-        <v>4</v>
-      </c>
-      <c r="F16">
-        <v>90</v>
-      </c>
-      <c r="G16">
-        <v>250</v>
-      </c>
-      <c r="H16">
-        <v>700</v>
-      </c>
-      <c r="I16">
-        <v>875</v>
-      </c>
-      <c r="J16">
-        <v>1050</v>
-      </c>
-      <c r="K16">
-        <v>150</v>
-      </c>
-      <c r="L16">
-        <v>110</v>
-      </c>
-      <c r="M16">
-        <v>121</v>
-      </c>
-      <c r="N16" s="9">
-        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17">
+        <v>37</v>
+      </c>
+      <c r="C17" s="10">
         <v>220</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="10">
         <v>18</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="10">
         <v>4</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="10">
         <v>90</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="10">
         <v>250</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="10">
         <v>700</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="10">
         <v>875</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="10">
         <v>1050</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="10">
         <v>150</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="10">
         <v>110</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="10">
         <v>121</v>
       </c>
       <c r="N17" s="9">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="10">
+        <v>220</v>
+      </c>
+      <c r="D18" s="10">
+        <v>18</v>
+      </c>
+      <c r="E18" s="10">
+        <v>4</v>
+      </c>
+      <c r="F18" s="10">
+        <v>90</v>
+      </c>
+      <c r="G18" s="10">
+        <v>250</v>
+      </c>
+      <c r="H18" s="10">
+        <v>700</v>
+      </c>
+      <c r="I18" s="10">
+        <v>875</v>
+      </c>
+      <c r="J18" s="10">
+        <v>1050</v>
+      </c>
+      <c r="K18" s="10">
+        <v>150</v>
+      </c>
+      <c r="L18" s="10">
+        <v>110</v>
+      </c>
+      <c r="M18" s="10">
+        <v>121</v>
+      </c>
+      <c r="N18" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C18">
+      <c r="C19" s="10">
         <v>240</v>
       </c>
-      <c r="D18">
+      <c r="D19" s="10">
         <v>20</v>
       </c>
-      <c r="E18">
+      <c r="E19" s="10">
         <v>4</v>
       </c>
-      <c r="F18">
+      <c r="F19" s="10">
         <v>100</v>
       </c>
-      <c r="G18">
+      <c r="G19" s="10">
         <v>300</v>
       </c>
-      <c r="H18">
+      <c r="H19" s="10">
         <v>750</v>
       </c>
-      <c r="I18">
+      <c r="I19" s="10">
         <v>925</v>
       </c>
-      <c r="J18">
+      <c r="J19" s="10">
         <v>1100</v>
       </c>
-      <c r="K18">
+      <c r="K19" s="10">
         <v>150</v>
       </c>
-      <c r="L18">
+      <c r="L19" s="10">
         <v>120</v>
       </c>
-      <c r="M18">
+      <c r="M19" s="10">
         <v>132</v>
       </c>
-      <c r="N18" s="9">
+      <c r="N19" s="9">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C19">
+      <c r="C20" s="10">
         <v>200</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F19">
+      <c r="F20" s="10">
         <v>25</v>
       </c>
-      <c r="G19">
+      <c r="G20" s="10">
         <v>50</v>
       </c>
-      <c r="H19">
+      <c r="H20" s="10">
         <v>100</v>
       </c>
-      <c r="I19">
+      <c r="I20" s="10">
         <v>200</v>
       </c>
-      <c r="L19">
+      <c r="L20" s="10">
         <v>100</v>
       </c>
-      <c r="M19">
+      <c r="M20" s="10">
         <v>110</v>
       </c>
-      <c r="N19" s="9">
+      <c r="N20" s="9">
         <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20">
-        <v>260</v>
-      </c>
-      <c r="D20">
-        <v>22</v>
-      </c>
-      <c r="E20">
-        <v>5</v>
-      </c>
-      <c r="F20">
-        <v>110</v>
-      </c>
-      <c r="G20">
-        <v>330</v>
-      </c>
-      <c r="H20">
-        <v>800</v>
-      </c>
-      <c r="I20">
-        <v>975</v>
-      </c>
-      <c r="J20">
-        <v>1150</v>
-      </c>
-      <c r="K20">
-        <v>150</v>
-      </c>
-      <c r="L20">
-        <v>130</v>
-      </c>
-      <c r="M20">
-        <v>143</v>
-      </c>
-      <c r="N20" s="9">
-        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="10">
+        <v>260</v>
+      </c>
+      <c r="D21" s="10">
+        <v>22</v>
+      </c>
+      <c r="E21" s="10">
+        <v>5</v>
+      </c>
+      <c r="F21" s="10">
+        <v>110</v>
+      </c>
+      <c r="G21" s="10">
+        <v>330</v>
+      </c>
+      <c r="H21" s="10">
+        <v>800</v>
+      </c>
+      <c r="I21" s="10">
+        <v>975</v>
+      </c>
+      <c r="J21" s="10">
+        <v>1150</v>
+      </c>
+      <c r="K21" s="10">
+        <v>150</v>
+      </c>
+      <c r="L21" s="10">
+        <v>130</v>
+      </c>
+      <c r="M21" s="10">
+        <v>143</v>
+      </c>
+      <c r="N21" s="9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B22" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C21">
+      <c r="C22" s="10">
         <v>260</v>
       </c>
-      <c r="D21">
+      <c r="D22" s="10">
         <v>22</v>
       </c>
-      <c r="E21">
+      <c r="E22" s="10">
         <v>5</v>
       </c>
-      <c r="F21">
+      <c r="F22" s="10">
         <v>110</v>
       </c>
-      <c r="G21">
+      <c r="G22" s="10">
         <v>330</v>
       </c>
-      <c r="H21">
+      <c r="H22" s="10">
         <v>800</v>
       </c>
-      <c r="I21">
+      <c r="I22" s="10">
         <v>975</v>
       </c>
-      <c r="J21">
+      <c r="J22" s="10">
         <v>1150</v>
       </c>
-      <c r="K21">
+      <c r="K22" s="10">
         <v>150</v>
       </c>
-      <c r="L21">
+      <c r="L22" s="10">
         <v>130</v>
       </c>
-      <c r="M21">
+      <c r="M22" s="10">
         <v>143</v>
       </c>
-      <c r="N21" s="9">
+      <c r="N22" s="9">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C22">
+      <c r="C23" s="10">
         <v>150</v>
       </c>
-      <c r="F22">
+      <c r="F23" s="10">
         <v>4</v>
       </c>
-      <c r="G22">
+      <c r="G23" s="10">
         <v>10</v>
       </c>
-      <c r="L22">
+      <c r="L23" s="10">
         <v>75</v>
       </c>
-      <c r="M22">
+      <c r="M23" s="10">
         <v>83</v>
       </c>
-      <c r="N22" s="9">
+      <c r="N23" s="9">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A23" s="8" t="s">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B24" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C23">
+      <c r="C24" s="10">
         <v>280</v>
       </c>
-      <c r="D23">
+      <c r="D24" s="10">
         <v>24</v>
       </c>
-      <c r="E23">
+      <c r="E24" s="10">
         <v>5</v>
       </c>
-      <c r="F23">
+      <c r="F24" s="10">
         <v>120</v>
       </c>
-      <c r="G23">
+      <c r="G24" s="10">
         <v>360</v>
       </c>
-      <c r="H23">
+      <c r="H24" s="10">
         <v>850</v>
       </c>
-      <c r="I23">
+      <c r="I24" s="10">
         <v>1025</v>
       </c>
-      <c r="J23">
+      <c r="J24" s="10">
         <v>1200</v>
       </c>
-      <c r="K23">
+      <c r="K24" s="10">
         <v>150</v>
       </c>
-      <c r="L23">
+      <c r="L24" s="10">
         <v>140</v>
       </c>
-      <c r="M23">
+      <c r="M24" s="10">
         <v>154</v>
       </c>
-      <c r="N23" s="9">
+      <c r="N24" s="9">
         <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24">
-        <v>300</v>
-      </c>
-      <c r="D24">
-        <v>26</v>
-      </c>
-      <c r="E24">
-        <v>6</v>
-      </c>
-      <c r="F24">
-        <v>130</v>
-      </c>
-      <c r="G24">
-        <v>390</v>
-      </c>
-      <c r="H24">
-        <v>900</v>
-      </c>
-      <c r="I24">
-        <v>1100</v>
-      </c>
-      <c r="J24">
-        <v>1275</v>
-      </c>
-      <c r="K24">
-        <v>200</v>
-      </c>
-      <c r="L24">
-        <v>150</v>
-      </c>
-      <c r="M24">
-        <v>165</v>
-      </c>
-      <c r="N24" s="9">
-        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25">
+        <v>51</v>
+      </c>
+      <c r="C25" s="10">
         <v>300</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="10">
         <v>26</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="10">
         <v>6</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="10">
         <v>130</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="10">
         <v>390</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="10">
         <v>900</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="10">
         <v>1100</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="10">
         <v>1275</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="10">
         <v>200</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="10">
         <v>150</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="10">
         <v>165</v>
       </c>
       <c r="N25" s="9">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="10">
+        <v>300</v>
+      </c>
+      <c r="D26" s="10">
+        <v>26</v>
+      </c>
+      <c r="E26" s="10">
+        <v>6</v>
+      </c>
+      <c r="F26" s="10">
+        <v>130</v>
+      </c>
+      <c r="G26" s="10">
+        <v>390</v>
+      </c>
+      <c r="H26" s="10">
+        <v>900</v>
+      </c>
+      <c r="I26" s="10">
+        <v>1100</v>
+      </c>
+      <c r="J26" s="10">
+        <v>1275</v>
+      </c>
+      <c r="K26" s="10">
+        <v>200</v>
+      </c>
+      <c r="L26" s="10">
+        <v>150</v>
+      </c>
+      <c r="M26" s="10">
+        <v>165</v>
+      </c>
+      <c r="N26" s="9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C26">
+      <c r="C27" s="10">
         <v>320</v>
       </c>
-      <c r="D26">
+      <c r="D27" s="10">
         <v>28</v>
       </c>
-      <c r="E26">
+      <c r="E27" s="10">
         <v>6</v>
       </c>
-      <c r="F26">
+      <c r="F27" s="10">
         <v>150</v>
       </c>
-      <c r="G26">
+      <c r="G27" s="10">
         <v>450</v>
       </c>
-      <c r="H26">
+      <c r="H27" s="10">
         <v>1000</v>
       </c>
-      <c r="I26">
+      <c r="I27" s="10">
         <v>1200</v>
       </c>
-      <c r="J26">
+      <c r="J27" s="10">
         <v>1400</v>
       </c>
-      <c r="K26">
+      <c r="K27" s="10">
         <v>200</v>
       </c>
-      <c r="L26">
+      <c r="L27" s="10">
         <v>160</v>
       </c>
-      <c r="M26">
+      <c r="M27" s="10">
         <v>176</v>
       </c>
-      <c r="N26" s="9">
+      <c r="N27" s="9">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C27">
+      <c r="C28" s="10">
         <v>200</v>
       </c>
-      <c r="F27">
+      <c r="F28" s="10">
         <v>25</v>
       </c>
-      <c r="G27">
+      <c r="G28" s="10">
         <v>50</v>
       </c>
-      <c r="H27">
+      <c r="H28" s="10">
         <v>100</v>
       </c>
-      <c r="I27">
+      <c r="I28" s="10">
         <v>200</v>
       </c>
-      <c r="L27">
+      <c r="L28" s="10">
         <v>100</v>
       </c>
-      <c r="M27">
+      <c r="M28" s="10">
         <v>110</v>
       </c>
-      <c r="N27" s="9">
+      <c r="N28" s="9">
         <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28">
-        <v>350</v>
-      </c>
-      <c r="D28">
-        <v>35</v>
-      </c>
-      <c r="E28">
-        <v>7</v>
-      </c>
-      <c r="F28">
-        <v>175</v>
-      </c>
-      <c r="G28">
-        <v>500</v>
-      </c>
-      <c r="H28">
-        <v>1100</v>
-      </c>
-      <c r="I28">
-        <v>1300</v>
-      </c>
-      <c r="J28">
-        <v>1500</v>
-      </c>
-      <c r="K28">
-        <v>200</v>
-      </c>
-      <c r="L28">
-        <v>175</v>
-      </c>
-      <c r="M28">
-        <v>193</v>
-      </c>
-      <c r="N28" s="9">
-        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="10">
+        <v>350</v>
+      </c>
+      <c r="D29" s="10">
+        <v>35</v>
+      </c>
+      <c r="E29" s="10">
+        <v>7</v>
+      </c>
+      <c r="F29" s="10">
+        <v>175</v>
+      </c>
+      <c r="G29" s="10">
+        <v>500</v>
+      </c>
+      <c r="H29" s="10">
+        <v>1100</v>
+      </c>
+      <c r="I29" s="10">
+        <v>1300</v>
+      </c>
+      <c r="J29" s="10">
+        <v>1500</v>
+      </c>
+      <c r="K29" s="10">
+        <v>200</v>
+      </c>
+      <c r="L29" s="10">
+        <v>175</v>
+      </c>
+      <c r="M29" s="10">
+        <v>193</v>
+      </c>
+      <c r="N29" s="9">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A30" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="10">
+        <v>100</v>
+      </c>
+      <c r="N30" s="9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C29">
+      <c r="C31" s="10">
         <v>400</v>
       </c>
-      <c r="D29">
+      <c r="D31" s="10">
         <v>50</v>
       </c>
-      <c r="E29">
+      <c r="E31" s="10">
         <v>7</v>
       </c>
-      <c r="F29">
+      <c r="F31" s="10">
         <v>200</v>
       </c>
-      <c r="G29">
+      <c r="G31" s="10">
         <v>600</v>
       </c>
-      <c r="H29">
+      <c r="H31" s="10">
         <v>1400</v>
       </c>
-      <c r="I29">
+      <c r="I31" s="10">
         <v>1700</v>
       </c>
-      <c r="J29">
+      <c r="J31" s="10">
         <v>2000</v>
       </c>
-      <c r="K29">
+      <c r="K31" s="10">
         <v>200</v>
       </c>
-      <c r="L29">
+      <c r="L31" s="10">
         <v>200</v>
       </c>
-      <c r="M29">
+      <c r="M31" s="10">
         <v>220</v>
       </c>
-      <c r="N29" s="9">
+      <c r="N31" s="9">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A32" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="N30" s="9">
+      <c r="N32" s="9">
         <v>40</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N32">
+    <sortCondition ref="N9:N32"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working on Jail. Add 3 turns+clean up
</commit_message>
<xml_diff>
--- a/resources/info.xlsx
+++ b/resources/info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\moi\programming things\0.projects\monopoly-discord-bot\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B231AFAB-08AD-4DC9-A9FB-83F2EB44A2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2673CC-F41E-4ADC-B0ED-47F09B17AAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="82">
   <si>
     <t>PropertyUS</t>
   </si>
@@ -229,13 +229,43 @@
     <t>Index</t>
   </si>
   <si>
-    <t>Get out of jail free</t>
-  </si>
-  <si>
     <t>Income Tax</t>
   </si>
   <si>
     <t>Super Tax</t>
+  </si>
+  <si>
+    <t>Emoji</t>
+  </si>
+  <si>
+    <t>:brown_square:</t>
+  </si>
+  <si>
+    <t>:blue_square:</t>
+  </si>
+  <si>
+    <t>:purple_square:</t>
+  </si>
+  <si>
+    <t>:orange_square:</t>
+  </si>
+  <si>
+    <t>:red_square:</t>
+  </si>
+  <si>
+    <t>:yellow_square:</t>
+  </si>
+  <si>
+    <t>:green_square:</t>
+  </si>
+  <si>
+    <t>:black_large_square:</t>
+  </si>
+  <si>
+    <t>:flag_white:</t>
+  </si>
+  <si>
+    <t>Get Out of Jail Free Card</t>
   </si>
 </sst>
 </file>
@@ -779,7 +809,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -790,9 +820,8 @@
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1160,1252 +1189,1349 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="11.54296875" style="10" customWidth="1"/>
-    <col min="3" max="13" width="6.08984375" style="10"/>
+    <col min="1" max="2" width="11.54296875" customWidth="1"/>
     <col min="14" max="14" width="6.08984375" style="9"/>
-    <col min="15" max="16384" width="6.08984375" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
       <c r="N1" s="9" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2">
         <v>60</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2">
         <v>2</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2">
         <v>10</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2">
         <v>30</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2">
         <v>90</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2">
         <v>160</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2">
         <v>250</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K2">
         <v>50</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2">
         <v>30</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2">
         <v>33</v>
       </c>
-      <c r="N2" s="13">
+      <c r="N2" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3">
         <v>60</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3">
         <v>4</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3">
         <v>20</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3">
         <v>60</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3">
         <v>180</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3">
         <v>320</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3">
         <v>450</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3">
         <v>50</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3">
         <v>30</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3">
         <v>33</v>
       </c>
       <c r="N3" s="9">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="10">
+      <c r="O3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4">
         <v>200</v>
+      </c>
+      <c r="E4">
+        <v>-2</v>
       </c>
       <c r="N4" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5">
         <v>200</v>
       </c>
-      <c r="F5" s="10">
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5">
         <v>25</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5">
         <v>50</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5">
         <v>100</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5">
         <v>200</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5">
         <v>100</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5">
         <v>110</v>
       </c>
       <c r="N5" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6">
         <v>100</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6">
         <v>6</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6">
         <v>30</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6">
         <v>90</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6">
         <v>270</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6">
         <v>400</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6">
         <v>550</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6">
         <v>50</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6">
         <v>50</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6">
         <v>55</v>
       </c>
       <c r="N6" s="9">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7">
         <v>100</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7">
         <v>6</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7">
         <v>30</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7">
         <v>90</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7">
         <v>270</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7">
         <v>400</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7">
         <v>550</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7">
         <v>50</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7">
         <v>50</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M7">
         <v>55</v>
       </c>
       <c r="N7" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8">
         <v>120</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8">
         <v>8</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8">
         <v>40</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8">
         <v>100</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8">
         <v>300</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8">
         <v>450</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8">
         <v>600</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8">
         <v>50</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8">
         <v>60</v>
       </c>
-      <c r="M8" s="10">
+      <c r="M8">
         <v>66</v>
       </c>
       <c r="N8" s="9">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9">
         <v>140</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9">
         <v>10</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9">
         <v>2</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9">
         <v>50</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9">
         <v>150</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9">
         <v>450</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9">
         <v>625</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9">
         <v>750</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9">
         <v>100</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9">
         <v>70</v>
       </c>
-      <c r="M9" s="10">
+      <c r="M9">
         <v>77</v>
       </c>
       <c r="N9" s="9">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
+      <c r="O9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10">
         <v>150</v>
       </c>
-      <c r="F10" s="10">
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10">
         <v>4</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10">
         <v>10</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10">
         <v>75</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10">
         <v>83</v>
       </c>
       <c r="N10" s="9">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11">
         <v>140</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11">
         <v>10</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11">
         <v>2</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11">
         <v>50</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11">
         <v>150</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11">
         <v>450</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11">
         <v>625</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11">
         <v>750</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11">
         <v>100</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11">
         <v>70</v>
       </c>
-      <c r="M11" s="10">
+      <c r="M11">
         <v>77</v>
       </c>
       <c r="N11" s="9">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12">
         <v>160</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12">
         <v>12</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12">
         <v>2</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12">
         <v>60</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12">
         <v>180</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12">
         <v>500</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12">
         <v>700</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12">
         <v>900</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12">
         <v>100</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12">
         <v>80</v>
       </c>
-      <c r="M12" s="10">
+      <c r="M12">
         <v>88</v>
       </c>
       <c r="N12" s="9">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
+      <c r="O12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13">
         <v>200</v>
       </c>
-      <c r="F13" s="10">
+      <c r="E13">
+        <v>8</v>
+      </c>
+      <c r="F13">
         <v>25</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13">
         <v>50</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13">
         <v>100</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13">
         <v>200</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13">
         <v>100</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M13">
         <v>110</v>
       </c>
       <c r="N13" s="9">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14">
         <v>180</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14">
         <v>14</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14">
         <v>3</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14">
         <v>70</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14">
         <v>200</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14">
         <v>550</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14">
         <v>750</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14">
         <v>950</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14">
         <v>100</v>
       </c>
-      <c r="L14" s="10">
+      <c r="L14">
         <v>90</v>
       </c>
-      <c r="M14" s="10">
+      <c r="M14">
         <v>99</v>
       </c>
       <c r="N14" s="9">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15">
         <v>180</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15">
         <v>14</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15">
         <v>3</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15">
         <v>70</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15">
         <v>200</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15">
         <v>550</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15">
         <v>750</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15">
         <v>950</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15">
         <v>100</v>
       </c>
-      <c r="L15" s="10">
+      <c r="L15">
         <v>90</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15">
         <v>99</v>
       </c>
       <c r="N15" s="9">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16">
         <v>200</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16">
         <v>16</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16">
         <v>3</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16">
         <v>80</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16">
         <v>220</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16">
         <v>600</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16">
         <v>800</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16">
         <v>1000</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16">
         <v>100</v>
       </c>
-      <c r="L16" s="10">
+      <c r="L16">
         <v>100</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16">
         <v>110</v>
       </c>
       <c r="N16" s="9">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17">
         <v>220</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17">
         <v>18</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17">
         <v>4</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17">
         <v>90</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G17">
         <v>250</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H17">
         <v>700</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17">
         <v>875</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17">
         <v>1050</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K17">
         <v>150</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L17">
         <v>110</v>
       </c>
-      <c r="M17" s="10">
+      <c r="M17">
         <v>121</v>
       </c>
       <c r="N17" s="9">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18">
         <v>220</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18">
         <v>18</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18">
         <v>4</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18">
         <v>90</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G18">
         <v>250</v>
       </c>
-      <c r="H18" s="10">
+      <c r="H18">
         <v>700</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18">
         <v>875</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18">
         <v>1050</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18">
         <v>150</v>
       </c>
-      <c r="L18" s="10">
+      <c r="L18">
         <v>110</v>
       </c>
-      <c r="M18" s="10">
+      <c r="M18">
         <v>121</v>
       </c>
       <c r="N18" s="9">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19">
         <v>240</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19">
         <v>20</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19">
         <v>4</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19">
         <v>100</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19">
         <v>300</v>
       </c>
-      <c r="H19" s="10">
+      <c r="H19">
         <v>750</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19">
         <v>925</v>
       </c>
-      <c r="J19" s="10">
+      <c r="J19">
         <v>1100</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19">
         <v>150</v>
       </c>
-      <c r="L19" s="10">
+      <c r="L19">
         <v>120</v>
       </c>
-      <c r="M19" s="10">
+      <c r="M19">
         <v>132</v>
       </c>
       <c r="N19" s="9">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="10" t="s">
+      <c r="O19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20">
         <v>200</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="10">
+      <c r="E20">
+        <v>8</v>
+      </c>
+      <c r="F20">
         <v>25</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G20">
         <v>50</v>
       </c>
-      <c r="H20" s="10">
+      <c r="H20">
         <v>100</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20">
         <v>200</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L20">
         <v>100</v>
       </c>
-      <c r="M20" s="10">
+      <c r="M20">
         <v>110</v>
       </c>
       <c r="N20" s="9">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="12" t="s">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A21" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21">
         <v>260</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21">
         <v>22</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21">
         <v>5</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21">
         <v>110</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G21">
         <v>330</v>
       </c>
-      <c r="H21" s="10">
+      <c r="H21">
         <v>800</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21">
         <v>975</v>
       </c>
-      <c r="J21" s="10">
+      <c r="J21">
         <v>1150</v>
       </c>
-      <c r="K21" s="10">
+      <c r="K21">
         <v>150</v>
       </c>
-      <c r="L21" s="10">
+      <c r="L21">
         <v>130</v>
       </c>
-      <c r="M21" s="10">
+      <c r="M21">
         <v>143</v>
       </c>
       <c r="N21" s="9">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" s="12" t="s">
+      <c r="O21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A22" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22">
         <v>260</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22">
         <v>22</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22">
         <v>5</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22">
         <v>110</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22">
         <v>330</v>
       </c>
-      <c r="H22" s="10">
+      <c r="H22">
         <v>800</v>
       </c>
-      <c r="I22" s="10">
+      <c r="I22">
         <v>975</v>
       </c>
-      <c r="J22" s="10">
+      <c r="J22">
         <v>1150</v>
       </c>
-      <c r="K22" s="10">
+      <c r="K22">
         <v>150</v>
       </c>
-      <c r="L22" s="10">
+      <c r="L22">
         <v>130</v>
       </c>
-      <c r="M22" s="10">
+      <c r="M22">
         <v>143</v>
       </c>
       <c r="N22" s="9">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A23" s="10" t="s">
+      <c r="O22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23">
         <v>150</v>
       </c>
-      <c r="F23" s="10">
+      <c r="E23">
+        <v>9</v>
+      </c>
+      <c r="F23">
         <v>4</v>
       </c>
-      <c r="G23" s="10">
+      <c r="G23">
         <v>10</v>
       </c>
-      <c r="L23" s="10">
+      <c r="L23">
         <v>75</v>
       </c>
-      <c r="M23" s="10">
+      <c r="M23">
         <v>83</v>
       </c>
       <c r="N23" s="9">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24">
         <v>280</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24">
         <v>24</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24">
         <v>5</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F24">
         <v>120</v>
       </c>
-      <c r="G24" s="10">
+      <c r="G24">
         <v>360</v>
       </c>
-      <c r="H24" s="10">
+      <c r="H24">
         <v>850</v>
       </c>
-      <c r="I24" s="10">
+      <c r="I24">
         <v>1025</v>
       </c>
-      <c r="J24" s="10">
+      <c r="J24">
         <v>1200</v>
       </c>
-      <c r="K24" s="10">
+      <c r="K24">
         <v>150</v>
       </c>
-      <c r="L24" s="10">
+      <c r="L24">
         <v>140</v>
       </c>
-      <c r="M24" s="10">
+      <c r="M24">
         <v>154</v>
       </c>
       <c r="N24" s="9">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25">
         <v>300</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25">
         <v>26</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25">
         <v>6</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F25">
         <v>130</v>
       </c>
-      <c r="G25" s="10">
+      <c r="G25">
         <v>390</v>
       </c>
-      <c r="H25" s="10">
+      <c r="H25">
         <v>900</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25">
         <v>1100</v>
       </c>
-      <c r="J25" s="10">
+      <c r="J25">
         <v>1275</v>
       </c>
-      <c r="K25" s="10">
+      <c r="K25">
         <v>200</v>
       </c>
-      <c r="L25" s="10">
+      <c r="L25">
         <v>150</v>
       </c>
-      <c r="M25" s="10">
+      <c r="M25">
         <v>165</v>
       </c>
       <c r="N25" s="9">
         <v>31</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26">
         <v>300</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26">
         <v>26</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26">
         <v>6</v>
       </c>
-      <c r="F26" s="10">
+      <c r="F26">
         <v>130</v>
       </c>
-      <c r="G26" s="10">
+      <c r="G26">
         <v>390</v>
       </c>
-      <c r="H26" s="10">
+      <c r="H26">
         <v>900</v>
       </c>
-      <c r="I26" s="10">
+      <c r="I26">
         <v>1100</v>
       </c>
-      <c r="J26" s="10">
+      <c r="J26">
         <v>1275</v>
       </c>
-      <c r="K26" s="10">
+      <c r="K26">
         <v>200</v>
       </c>
-      <c r="L26" s="10">
+      <c r="L26">
         <v>150</v>
       </c>
-      <c r="M26" s="10">
+      <c r="M26">
         <v>165</v>
       </c>
       <c r="N26" s="9">
         <v>32</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27">
         <v>320</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27">
         <v>28</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27">
         <v>6</v>
       </c>
-      <c r="F27" s="10">
+      <c r="F27">
         <v>150</v>
       </c>
-      <c r="G27" s="10">
+      <c r="G27">
         <v>450</v>
       </c>
-      <c r="H27" s="10">
+      <c r="H27">
         <v>1000</v>
       </c>
-      <c r="I27" s="10">
+      <c r="I27">
         <v>1200</v>
       </c>
-      <c r="J27" s="10">
+      <c r="J27">
         <v>1400</v>
       </c>
-      <c r="K27" s="10">
+      <c r="K27">
         <v>200</v>
       </c>
-      <c r="L27" s="10">
+      <c r="L27">
         <v>160</v>
       </c>
-      <c r="M27" s="10">
+      <c r="M27">
         <v>176</v>
       </c>
       <c r="N27" s="9">
         <v>34</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A28" s="10" t="s">
+      <c r="O27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28">
         <v>200</v>
       </c>
-      <c r="F28" s="10">
+      <c r="E28">
+        <v>8</v>
+      </c>
+      <c r="F28">
         <v>25</v>
       </c>
-      <c r="G28" s="10">
+      <c r="G28">
         <v>50</v>
       </c>
-      <c r="H28" s="10">
+      <c r="H28">
         <v>100</v>
       </c>
-      <c r="I28" s="10">
+      <c r="I28">
         <v>200</v>
       </c>
-      <c r="L28" s="10">
+      <c r="L28">
         <v>100</v>
       </c>
-      <c r="M28" s="10">
+      <c r="M28">
         <v>110</v>
       </c>
       <c r="N28" s="9">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29">
         <v>350</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29">
         <v>35</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29">
         <v>7</v>
       </c>
-      <c r="F29" s="10">
+      <c r="F29">
         <v>175</v>
       </c>
-      <c r="G29" s="10">
+      <c r="G29">
         <v>500</v>
       </c>
-      <c r="H29" s="10">
+      <c r="H29">
         <v>1100</v>
       </c>
-      <c r="I29" s="10">
+      <c r="I29">
         <v>1300</v>
       </c>
-      <c r="J29" s="10">
+      <c r="J29">
         <v>1500</v>
       </c>
-      <c r="K29" s="10">
+      <c r="K29">
         <v>200</v>
       </c>
-      <c r="L29" s="10">
+      <c r="L29">
         <v>175</v>
       </c>
-      <c r="M29" s="10">
+      <c r="M29">
         <v>193</v>
       </c>
       <c r="N29" s="9">
         <v>37</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A30" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="10">
+      <c r="O29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A30" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30">
         <v>100</v>
+      </c>
+      <c r="E30">
+        <v>-2</v>
       </c>
       <c r="N30" s="9">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C31">
         <v>400</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D31">
         <v>50</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E31">
         <v>7</v>
       </c>
-      <c r="F31" s="10">
+      <c r="F31">
         <v>200</v>
       </c>
-      <c r="G31" s="10">
+      <c r="G31">
         <v>600</v>
       </c>
-      <c r="H31" s="10">
+      <c r="H31">
         <v>1400</v>
       </c>
-      <c r="I31" s="10">
+      <c r="I31">
         <v>1700</v>
       </c>
-      <c r="J31" s="10">
+      <c r="J31">
         <v>2000</v>
       </c>
-      <c r="K31" s="10">
+      <c r="K31">
         <v>200</v>
       </c>
-      <c r="L31" s="10">
+      <c r="L31">
         <v>200</v>
       </c>
-      <c r="M31" s="10">
+      <c r="M31">
         <v>220</v>
       </c>
       <c r="N31" s="9">
         <v>39</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A32" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>69</v>
+      <c r="O31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32">
+        <v>-1</v>
       </c>
       <c r="N32" s="9">
         <v>40</v>
+      </c>
+      <c r="O32" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Retired index() everything is now extracted from info.csv
</commit_message>
<xml_diff>
--- a/resources/info.xlsx
+++ b/resources/info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\moi\programming things\0.projects\monopoly-discord-bot\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2673CC-F41E-4ADC-B0ED-47F09B17AAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA62C37-0DD0-43B1-9AFA-A4D1DA4BA72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="88">
   <si>
     <t>PropertyUS</t>
   </si>
@@ -266,6 +266,24 @@
   </si>
   <si>
     <t>Get Out of Jail Free Card</t>
+  </si>
+  <si>
+    <t>Community Chest</t>
+  </si>
+  <si>
+    <t>Chance</t>
+  </si>
+  <si>
+    <t>Free Parking</t>
+  </si>
+  <si>
+    <t>Go To Jail</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Just Visiting Jail</t>
   </si>
 </sst>
 </file>
@@ -414,7 +432,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="42">
+  <fills count="48">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -602,12 +620,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF0099CC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -645,6 +657,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -809,22 +863,33 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1189,19 +1254,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="7.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="11.54296875" customWidth="1"/>
-    <col min="14" max="14" width="6.08984375" style="9"/>
+    <col min="1" max="2" width="18.90625" customWidth="1"/>
+    <col min="14" max="14" width="7.36328125" style="9"/>
+    <col min="15" max="15" width="14.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1247,8 +1313,11 @@
       <c r="O1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -1288,165 +1357,144 @@
       <c r="M2">
         <v>33</v>
       </c>
-      <c r="N2" s="12">
+      <c r="N2" s="11">
         <v>1</v>
       </c>
       <c r="O2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+      <c r="P2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="N3" s="11">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>60</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>4</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="F4">
         <v>20</v>
       </c>
-      <c r="G3">
+      <c r="G4">
         <v>60</v>
       </c>
-      <c r="H3">
+      <c r="H4">
         <v>180</v>
       </c>
-      <c r="I3">
+      <c r="I4">
         <v>320</v>
       </c>
-      <c r="J3">
+      <c r="J4">
         <v>450</v>
       </c>
-      <c r="K3">
+      <c r="K4">
         <v>50</v>
       </c>
-      <c r="L3">
+      <c r="L4">
         <v>30</v>
       </c>
-      <c r="M3">
+      <c r="M4">
         <v>33</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N4" s="9">
         <v>3</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="P4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="15" t="s">
         <v>69</v>
-      </c>
-      <c r="C4">
-        <v>200</v>
-      </c>
-      <c r="E4">
-        <v>-2</v>
-      </c>
-      <c r="N4" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>14</v>
       </c>
       <c r="C5">
         <v>200</v>
       </c>
       <c r="E5">
+        <v>-2</v>
+      </c>
+      <c r="N5" s="9">
+        <v>4</v>
+      </c>
+      <c r="P5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>200</v>
+      </c>
+      <c r="E6">
         <v>8</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>25</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <v>50</v>
       </c>
-      <c r="H5">
+      <c r="H6">
         <v>100</v>
       </c>
-      <c r="I5">
+      <c r="I6">
         <v>200</v>
       </c>
-      <c r="L5">
+      <c r="L6">
         <v>100</v>
       </c>
-      <c r="M5">
+      <c r="M6">
         <v>110</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N6" s="9">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+      <c r="P6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B7" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="C6">
-        <v>100</v>
-      </c>
-      <c r="D6">
-        <v>6</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>30</v>
-      </c>
-      <c r="G6">
-        <v>90</v>
-      </c>
-      <c r="H6">
-        <v>270</v>
-      </c>
-      <c r="I6">
-        <v>400</v>
-      </c>
-      <c r="J6">
-        <v>550</v>
-      </c>
-      <c r="K6">
-        <v>50</v>
-      </c>
-      <c r="L6">
-        <v>50</v>
-      </c>
-      <c r="M6">
-        <v>55</v>
-      </c>
-      <c r="N6" s="9">
-        <v>6</v>
-      </c>
-      <c r="O6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="C7">
         <v>100</v>
@@ -1482,391 +1530,349 @@
         <v>55</v>
       </c>
       <c r="N7" s="9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O7" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+      <c r="P7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="N8" s="11">
+        <v>7</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>30</v>
+      </c>
+      <c r="G9">
+        <v>90</v>
+      </c>
+      <c r="H9">
+        <v>270</v>
+      </c>
+      <c r="I9">
+        <v>400</v>
+      </c>
+      <c r="J9">
+        <v>550</v>
+      </c>
+      <c r="K9">
+        <v>50</v>
+      </c>
+      <c r="L9">
+        <v>50</v>
+      </c>
+      <c r="M9">
+        <v>55</v>
+      </c>
+      <c r="N9" s="11">
+        <v>8</v>
+      </c>
+      <c r="O9" t="s">
+        <v>73</v>
+      </c>
+      <c r="P9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C8">
+      <c r="C10">
         <v>120</v>
       </c>
-      <c r="D8">
+      <c r="D10">
         <v>8</v>
       </c>
-      <c r="E8">
+      <c r="E10">
         <v>1</v>
       </c>
-      <c r="F8">
+      <c r="F10">
         <v>40</v>
       </c>
-      <c r="G8">
+      <c r="G10">
         <v>100</v>
       </c>
-      <c r="H8">
+      <c r="H10">
         <v>300</v>
       </c>
-      <c r="I8">
+      <c r="I10">
         <v>450</v>
       </c>
-      <c r="J8">
+      <c r="J10">
         <v>600</v>
       </c>
-      <c r="K8">
+      <c r="K10">
         <v>50</v>
       </c>
-      <c r="L8">
+      <c r="L10">
         <v>60</v>
       </c>
-      <c r="M8">
+      <c r="M10">
         <v>66</v>
       </c>
-      <c r="N8" s="9">
+      <c r="N10" s="9">
         <v>9</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="P10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="N11" s="9">
+        <v>10</v>
+      </c>
+      <c r="P11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C9">
+      <c r="C12">
         <v>140</v>
       </c>
-      <c r="D9">
+      <c r="D12">
         <v>10</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>50</v>
-      </c>
-      <c r="G9">
-        <v>150</v>
-      </c>
-      <c r="H9">
-        <v>450</v>
-      </c>
-      <c r="I9">
-        <v>625</v>
-      </c>
-      <c r="J9">
-        <v>750</v>
-      </c>
-      <c r="K9">
-        <v>100</v>
-      </c>
-      <c r="L9">
-        <v>70</v>
-      </c>
-      <c r="M9">
-        <v>77</v>
-      </c>
-      <c r="N9" s="9">
-        <v>11</v>
-      </c>
-      <c r="O9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10">
-        <v>150</v>
-      </c>
-      <c r="E10">
-        <v>9</v>
-      </c>
-      <c r="F10">
-        <v>4</v>
-      </c>
-      <c r="G10">
-        <v>10</v>
-      </c>
-      <c r="L10">
-        <v>75</v>
-      </c>
-      <c r="M10">
-        <v>83</v>
-      </c>
-      <c r="N10" s="9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11">
-        <v>140</v>
-      </c>
-      <c r="D11">
-        <v>10</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>50</v>
-      </c>
-      <c r="G11">
-        <v>150</v>
-      </c>
-      <c r="H11">
-        <v>450</v>
-      </c>
-      <c r="I11">
-        <v>625</v>
-      </c>
-      <c r="J11">
-        <v>750</v>
-      </c>
-      <c r="K11">
-        <v>100</v>
-      </c>
-      <c r="L11">
-        <v>70</v>
-      </c>
-      <c r="M11">
-        <v>77</v>
-      </c>
-      <c r="N11" s="9">
-        <v>13</v>
-      </c>
-      <c r="O11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12">
-        <v>160</v>
-      </c>
-      <c r="D12">
-        <v>12</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
       <c r="F12">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G12">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="H12">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="I12">
-        <v>700</v>
+        <v>625</v>
       </c>
       <c r="J12">
-        <v>900</v>
+        <v>750</v>
       </c>
       <c r="K12">
         <v>100</v>
       </c>
       <c r="L12">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="M12">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="N12" s="9">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="O12" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" t="s">
-        <v>62</v>
+      <c r="P12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>23</v>
       </c>
       <c r="C13">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E13">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+      <c r="L13">
+        <v>75</v>
+      </c>
+      <c r="M13">
+        <v>83</v>
+      </c>
+      <c r="N13" s="9">
+        <v>12</v>
+      </c>
+      <c r="P13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G13">
+      <c r="B14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14">
+        <v>140</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
         <v>50</v>
       </c>
-      <c r="H13">
-        <v>100</v>
-      </c>
-      <c r="I13">
-        <v>200</v>
-      </c>
-      <c r="L13">
-        <v>100</v>
-      </c>
-      <c r="M13">
-        <v>110</v>
-      </c>
-      <c r="N13" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14">
-        <v>180</v>
-      </c>
-      <c r="D14">
-        <v>14</v>
-      </c>
-      <c r="E14">
-        <v>3</v>
-      </c>
-      <c r="F14">
-        <v>70</v>
-      </c>
       <c r="G14">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="H14">
-        <v>550</v>
+        <v>450</v>
       </c>
       <c r="I14">
+        <v>625</v>
+      </c>
+      <c r="J14">
         <v>750</v>
-      </c>
-      <c r="J14">
-        <v>950</v>
       </c>
       <c r="K14">
         <v>100</v>
       </c>
       <c r="L14">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="M14">
-        <v>99</v>
-      </c>
-      <c r="N14" s="9">
-        <v>16</v>
+        <v>77</v>
+      </c>
+      <c r="N14" s="11">
+        <v>13</v>
       </c>
       <c r="O14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>33</v>
+        <v>74</v>
+      </c>
+      <c r="P14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="C15">
+        <v>160</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>60</v>
+      </c>
+      <c r="G15">
         <v>180</v>
       </c>
-      <c r="D15">
-        <v>14</v>
-      </c>
-      <c r="E15">
-        <v>3</v>
-      </c>
-      <c r="F15">
-        <v>70</v>
-      </c>
-      <c r="G15">
-        <v>200</v>
-      </c>
       <c r="H15">
-        <v>550</v>
+        <v>500</v>
       </c>
       <c r="I15">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="J15">
-        <v>950</v>
+        <v>900</v>
       </c>
       <c r="K15">
         <v>100</v>
       </c>
       <c r="L15">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="M15">
-        <v>99</v>
-      </c>
-      <c r="N15" s="9">
-        <v>18</v>
+        <v>88</v>
+      </c>
+      <c r="N15" s="11">
+        <v>14</v>
       </c>
       <c r="O15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>74</v>
+      </c>
+      <c r="P15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A16" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>62</v>
       </c>
       <c r="C16">
         <v>200</v>
       </c>
-      <c r="D16">
-        <v>16</v>
-      </c>
       <c r="E16">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F16">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="G16">
-        <v>220</v>
+        <v>50</v>
       </c>
       <c r="H16">
-        <v>600</v>
+        <v>100</v>
       </c>
       <c r="I16">
-        <v>800</v>
-      </c>
-      <c r="J16">
-        <v>1000</v>
-      </c>
-      <c r="K16">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="L16">
         <v>100</v>
@@ -1875,180 +1881,159 @@
         <v>110</v>
       </c>
       <c r="N16" s="9">
-        <v>19</v>
-      </c>
-      <c r="O16" t="s">
+        <v>15</v>
+      </c>
+      <c r="P16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17">
+        <v>180</v>
+      </c>
+      <c r="D17">
+        <v>14</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>70</v>
+      </c>
+      <c r="G17">
+        <v>200</v>
+      </c>
+      <c r="H17">
+        <v>550</v>
+      </c>
+      <c r="I17">
+        <v>750</v>
+      </c>
+      <c r="J17">
+        <v>950</v>
+      </c>
+      <c r="K17">
+        <v>100</v>
+      </c>
+      <c r="L17">
+        <v>90</v>
+      </c>
+      <c r="M17">
+        <v>99</v>
+      </c>
+      <c r="N17" s="9">
+        <v>16</v>
+      </c>
+      <c r="O17" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17">
-        <v>220</v>
-      </c>
-      <c r="D17">
+      <c r="P17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A18" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="N18" s="9">
+        <v>17</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19">
+        <v>180</v>
+      </c>
+      <c r="D19">
+        <v>14</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>70</v>
+      </c>
+      <c r="G19">
+        <v>200</v>
+      </c>
+      <c r="H19">
+        <v>550</v>
+      </c>
+      <c r="I19">
+        <v>750</v>
+      </c>
+      <c r="J19">
+        <v>950</v>
+      </c>
+      <c r="K19">
+        <v>100</v>
+      </c>
+      <c r="L19">
+        <v>90</v>
+      </c>
+      <c r="M19">
+        <v>99</v>
+      </c>
+      <c r="N19" s="9">
         <v>18</v>
       </c>
-      <c r="E17">
-        <v>4</v>
-      </c>
-      <c r="F17">
-        <v>90</v>
-      </c>
-      <c r="G17">
-        <v>250</v>
-      </c>
-      <c r="H17">
-        <v>700</v>
-      </c>
-      <c r="I17">
-        <v>875</v>
-      </c>
-      <c r="J17">
-        <v>1050</v>
-      </c>
-      <c r="K17">
-        <v>150</v>
-      </c>
-      <c r="L17">
-        <v>110</v>
-      </c>
-      <c r="M17">
-        <v>121</v>
-      </c>
-      <c r="N17" s="9">
-        <v>21</v>
-      </c>
-      <c r="O17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18">
-        <v>220</v>
-      </c>
-      <c r="D18">
-        <v>18</v>
-      </c>
-      <c r="E18">
-        <v>4</v>
-      </c>
-      <c r="F18">
-        <v>90</v>
-      </c>
-      <c r="G18">
-        <v>250</v>
-      </c>
-      <c r="H18">
-        <v>700</v>
-      </c>
-      <c r="I18">
-        <v>875</v>
-      </c>
-      <c r="J18">
-        <v>1050</v>
-      </c>
-      <c r="K18">
-        <v>150</v>
-      </c>
-      <c r="L18">
-        <v>110</v>
-      </c>
-      <c r="M18">
-        <v>121</v>
-      </c>
-      <c r="N18" s="9">
-        <v>23</v>
-      </c>
-      <c r="O18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19">
-        <v>240</v>
-      </c>
-      <c r="D19">
-        <v>20</v>
-      </c>
-      <c r="E19">
-        <v>4</v>
-      </c>
-      <c r="F19">
-        <v>100</v>
-      </c>
-      <c r="G19">
-        <v>300</v>
-      </c>
-      <c r="H19">
-        <v>750</v>
-      </c>
-      <c r="I19">
-        <v>925</v>
-      </c>
-      <c r="J19">
-        <v>1100</v>
-      </c>
-      <c r="K19">
-        <v>150</v>
-      </c>
-      <c r="L19">
-        <v>120</v>
-      </c>
-      <c r="M19">
-        <v>132</v>
-      </c>
-      <c r="N19" s="9">
-        <v>24</v>
-      </c>
       <c r="O19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" t="s">
-        <v>63</v>
+        <v>75</v>
+      </c>
+      <c r="P19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="C20">
         <v>200</v>
       </c>
-      <c r="D20" t="s">
-        <v>24</v>
+      <c r="D20">
+        <v>16</v>
       </c>
       <c r="E20">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F20">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="G20">
-        <v>50</v>
+        <v>220</v>
       </c>
       <c r="H20">
+        <v>600</v>
+      </c>
+      <c r="I20">
+        <v>800</v>
+      </c>
+      <c r="J20">
+        <v>1000</v>
+      </c>
+      <c r="K20">
         <v>100</v>
-      </c>
-      <c r="I20">
-        <v>200</v>
       </c>
       <c r="L20">
         <v>100</v>
@@ -2056,487 +2041,790 @@
       <c r="M20">
         <v>110</v>
       </c>
-      <c r="N20" s="9">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21">
-        <v>260</v>
-      </c>
-      <c r="D21">
-        <v>22</v>
-      </c>
-      <c r="E21">
-        <v>5</v>
-      </c>
-      <c r="F21">
-        <v>110</v>
-      </c>
-      <c r="G21">
-        <v>330</v>
-      </c>
-      <c r="H21">
-        <v>800</v>
-      </c>
-      <c r="I21">
-        <v>975</v>
-      </c>
-      <c r="J21">
-        <v>1150</v>
-      </c>
-      <c r="K21">
-        <v>150</v>
-      </c>
-      <c r="L21">
-        <v>130</v>
-      </c>
-      <c r="M21">
-        <v>143</v>
-      </c>
-      <c r="N21" s="9">
-        <v>26</v>
-      </c>
-      <c r="O21" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>46</v>
+      <c r="N20" s="11">
+        <v>19</v>
+      </c>
+      <c r="O20" t="s">
+        <v>75</v>
+      </c>
+      <c r="P20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="N21" s="11">
+        <v>20</v>
+      </c>
+      <c r="P21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="C22">
-        <v>260</v>
+        <v>220</v>
       </c>
       <c r="D22">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="G22">
-        <v>330</v>
+        <v>250</v>
       </c>
       <c r="H22">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="I22">
-        <v>975</v>
+        <v>875</v>
       </c>
       <c r="J22">
-        <v>1150</v>
+        <v>1050</v>
       </c>
       <c r="K22">
         <v>150</v>
       </c>
       <c r="L22">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="M22">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="N22" s="9">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="O22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23">
-        <v>150</v>
-      </c>
-      <c r="E23">
-        <v>9</v>
-      </c>
-      <c r="F23">
+        <v>76</v>
+      </c>
+      <c r="P22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="N23" s="11">
+        <v>22</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24">
+        <v>220</v>
+      </c>
+      <c r="D24">
+        <v>18</v>
+      </c>
+      <c r="E24">
         <v>4</v>
       </c>
-      <c r="G23">
-        <v>10</v>
-      </c>
-      <c r="L23">
-        <v>75</v>
-      </c>
-      <c r="M23">
-        <v>83</v>
-      </c>
-      <c r="N23" s="9">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A24" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24">
-        <v>280</v>
-      </c>
-      <c r="D24">
-        <v>24</v>
-      </c>
-      <c r="E24">
-        <v>5</v>
-      </c>
       <c r="F24">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="G24">
-        <v>360</v>
+        <v>250</v>
       </c>
       <c r="H24">
-        <v>850</v>
+        <v>700</v>
       </c>
       <c r="I24">
-        <v>1025</v>
+        <v>875</v>
       </c>
       <c r="J24">
-        <v>1200</v>
+        <v>1050</v>
       </c>
       <c r="K24">
         <v>150</v>
       </c>
       <c r="L24">
+        <v>110</v>
+      </c>
+      <c r="M24">
+        <v>121</v>
+      </c>
+      <c r="N24" s="11">
+        <v>23</v>
+      </c>
+      <c r="O24" t="s">
+        <v>76</v>
+      </c>
+      <c r="P24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25">
+        <v>240</v>
+      </c>
+      <c r="D25">
+        <v>20</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+      <c r="F25">
+        <v>100</v>
+      </c>
+      <c r="G25">
+        <v>300</v>
+      </c>
+      <c r="H25">
+        <v>750</v>
+      </c>
+      <c r="I25">
+        <v>925</v>
+      </c>
+      <c r="J25">
+        <v>1100</v>
+      </c>
+      <c r="K25">
+        <v>150</v>
+      </c>
+      <c r="L25">
+        <v>120</v>
+      </c>
+      <c r="M25">
+        <v>132</v>
+      </c>
+      <c r="N25" s="9">
+        <v>24</v>
+      </c>
+      <c r="O25" t="s">
+        <v>76</v>
+      </c>
+      <c r="P25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A26" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26">
+        <v>200</v>
+      </c>
+      <c r="D26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26">
+        <v>8</v>
+      </c>
+      <c r="F26">
+        <v>25</v>
+      </c>
+      <c r="G26">
+        <v>50</v>
+      </c>
+      <c r="H26">
+        <v>100</v>
+      </c>
+      <c r="I26">
+        <v>200</v>
+      </c>
+      <c r="L26">
+        <v>100</v>
+      </c>
+      <c r="M26">
+        <v>110</v>
+      </c>
+      <c r="N26" s="9">
+        <v>25</v>
+      </c>
+      <c r="P26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A27" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27">
+        <v>260</v>
+      </c>
+      <c r="D27">
+        <v>22</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <v>110</v>
+      </c>
+      <c r="G27">
+        <v>330</v>
+      </c>
+      <c r="H27">
+        <v>800</v>
+      </c>
+      <c r="I27">
+        <v>975</v>
+      </c>
+      <c r="J27">
+        <v>1150</v>
+      </c>
+      <c r="K27">
+        <v>150</v>
+      </c>
+      <c r="L27">
+        <v>130</v>
+      </c>
+      <c r="M27">
+        <v>143</v>
+      </c>
+      <c r="N27" s="9">
+        <v>26</v>
+      </c>
+      <c r="O27" t="s">
+        <v>77</v>
+      </c>
+      <c r="P27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A28" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28">
+        <v>260</v>
+      </c>
+      <c r="D28">
+        <v>22</v>
+      </c>
+      <c r="E28">
+        <v>5</v>
+      </c>
+      <c r="F28">
+        <v>110</v>
+      </c>
+      <c r="G28">
+        <v>330</v>
+      </c>
+      <c r="H28">
+        <v>800</v>
+      </c>
+      <c r="I28">
+        <v>975</v>
+      </c>
+      <c r="J28">
+        <v>1150</v>
+      </c>
+      <c r="K28">
+        <v>150</v>
+      </c>
+      <c r="L28">
+        <v>130</v>
+      </c>
+      <c r="M28">
+        <v>143</v>
+      </c>
+      <c r="N28" s="9">
+        <v>27</v>
+      </c>
+      <c r="O28" t="s">
+        <v>77</v>
+      </c>
+      <c r="P28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A29" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29">
+        <v>150</v>
+      </c>
+      <c r="E29">
+        <v>9</v>
+      </c>
+      <c r="F29">
+        <v>4</v>
+      </c>
+      <c r="G29">
+        <v>10</v>
+      </c>
+      <c r="L29">
+        <v>75</v>
+      </c>
+      <c r="M29">
+        <v>83</v>
+      </c>
+      <c r="N29" s="11">
+        <v>28</v>
+      </c>
+      <c r="P29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A30" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30">
+        <v>280</v>
+      </c>
+      <c r="D30">
+        <v>24</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
+      <c r="F30">
+        <v>120</v>
+      </c>
+      <c r="G30">
+        <v>360</v>
+      </c>
+      <c r="H30">
+        <v>850</v>
+      </c>
+      <c r="I30">
+        <v>1025</v>
+      </c>
+      <c r="J30">
+        <v>1200</v>
+      </c>
+      <c r="K30">
+        <v>150</v>
+      </c>
+      <c r="L30">
         <v>140</v>
       </c>
-      <c r="M24">
+      <c r="M30">
         <v>154</v>
       </c>
-      <c r="N24" s="9">
+      <c r="N30" s="11">
         <v>29</v>
       </c>
-      <c r="O24" t="s">
+      <c r="O30" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
+      <c r="P30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A31" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="N31" s="9">
+        <v>30</v>
+      </c>
+      <c r="P31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C25">
+      <c r="C32">
         <v>300</v>
       </c>
-      <c r="D25">
+      <c r="D32">
         <v>26</v>
       </c>
-      <c r="E25">
+      <c r="E32">
         <v>6</v>
       </c>
-      <c r="F25">
+      <c r="F32">
         <v>130</v>
       </c>
-      <c r="G25">
+      <c r="G32">
         <v>390</v>
       </c>
-      <c r="H25">
+      <c r="H32">
         <v>900</v>
       </c>
-      <c r="I25">
+      <c r="I32">
         <v>1100</v>
       </c>
-      <c r="J25">
+      <c r="J32">
         <v>1275</v>
       </c>
-      <c r="K25">
+      <c r="K32">
         <v>200</v>
       </c>
-      <c r="L25">
+      <c r="L32">
         <v>150</v>
       </c>
-      <c r="M25">
+      <c r="M32">
         <v>165</v>
       </c>
-      <c r="N25" s="9">
+      <c r="N32" s="9">
         <v>31</v>
       </c>
-      <c r="O25" t="s">
+      <c r="O32" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
+      <c r="P32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C26">
+      <c r="C33">
         <v>300</v>
       </c>
-      <c r="D26">
+      <c r="D33">
         <v>26</v>
       </c>
-      <c r="E26">
+      <c r="E33">
         <v>6</v>
       </c>
-      <c r="F26">
+      <c r="F33">
         <v>130</v>
       </c>
-      <c r="G26">
+      <c r="G33">
         <v>390</v>
       </c>
-      <c r="H26">
+      <c r="H33">
         <v>900</v>
       </c>
-      <c r="I26">
+      <c r="I33">
         <v>1100</v>
       </c>
-      <c r="J26">
+      <c r="J33">
         <v>1275</v>
       </c>
-      <c r="K26">
+      <c r="K33">
         <v>200</v>
       </c>
-      <c r="L26">
+      <c r="L33">
         <v>150</v>
       </c>
-      <c r="M26">
+      <c r="M33">
         <v>165</v>
       </c>
-      <c r="N26" s="9">
+      <c r="N33" s="9">
         <v>32</v>
       </c>
-      <c r="O26" t="s">
+      <c r="O33" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
+      <c r="P33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A34" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="N34" s="9">
+        <v>33</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C27">
+      <c r="C35">
         <v>320</v>
       </c>
-      <c r="D27">
+      <c r="D35">
         <v>28</v>
       </c>
-      <c r="E27">
+      <c r="E35">
         <v>6</v>
       </c>
-      <c r="F27">
+      <c r="F35">
         <v>150</v>
       </c>
-      <c r="G27">
+      <c r="G35">
         <v>450</v>
       </c>
-      <c r="H27">
+      <c r="H35">
         <v>1000</v>
       </c>
-      <c r="I27">
+      <c r="I35">
         <v>1200</v>
       </c>
-      <c r="J27">
+      <c r="J35">
         <v>1400</v>
       </c>
-      <c r="K27">
+      <c r="K35">
         <v>200</v>
       </c>
-      <c r="L27">
+      <c r="L35">
         <v>160</v>
       </c>
-      <c r="M27">
+      <c r="M35">
         <v>176</v>
       </c>
-      <c r="N27" s="9">
+      <c r="N35" s="11">
         <v>34</v>
       </c>
-      <c r="O27" t="s">
+      <c r="O35" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="P35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A36" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B36" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C28">
+      <c r="C36">
         <v>200</v>
       </c>
-      <c r="E28">
+      <c r="E36">
         <v>8</v>
       </c>
-      <c r="F28">
+      <c r="F36">
         <v>25</v>
       </c>
-      <c r="G28">
+      <c r="G36">
         <v>50</v>
       </c>
-      <c r="H28">
+      <c r="H36">
         <v>100</v>
       </c>
-      <c r="I28">
+      <c r="I36">
         <v>200</v>
       </c>
-      <c r="L28">
+      <c r="L36">
         <v>100</v>
       </c>
-      <c r="M28">
+      <c r="M36">
         <v>110</v>
       </c>
-      <c r="N28" s="9">
+      <c r="N36" s="11">
         <v>35</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
+      <c r="P36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A37" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="N37" s="9">
+        <v>36</v>
+      </c>
+      <c r="P37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C29">
+      <c r="C38">
         <v>350</v>
       </c>
-      <c r="D29">
+      <c r="D38">
         <v>35</v>
       </c>
-      <c r="E29">
+      <c r="E38">
         <v>7</v>
       </c>
-      <c r="F29">
+      <c r="F38">
         <v>175</v>
       </c>
-      <c r="G29">
+      <c r="G38">
         <v>500</v>
       </c>
-      <c r="H29">
+      <c r="H38">
         <v>1100</v>
       </c>
-      <c r="I29">
+      <c r="I38">
         <v>1300</v>
       </c>
-      <c r="J29">
+      <c r="J38">
         <v>1500</v>
       </c>
-      <c r="K29">
+      <c r="K38">
         <v>200</v>
       </c>
-      <c r="L29">
+      <c r="L38">
         <v>175</v>
       </c>
-      <c r="M29">
+      <c r="M38">
         <v>193</v>
       </c>
-      <c r="N29" s="9">
+      <c r="N38" s="9">
         <v>37</v>
       </c>
-      <c r="O29" t="s">
+      <c r="O38" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A30" s="12" t="s">
+      <c r="P38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A39" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B39" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="C30">
+      <c r="C39">
         <v>100</v>
       </c>
-      <c r="E30">
+      <c r="E39">
         <v>-2</v>
       </c>
-      <c r="N30" s="9">
+      <c r="N39" s="9">
         <v>38</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+      <c r="P39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C31">
+      <c r="C40">
         <v>400</v>
       </c>
-      <c r="D31">
+      <c r="D40">
         <v>50</v>
       </c>
-      <c r="E31">
+      <c r="E40">
         <v>7</v>
       </c>
-      <c r="F31">
+      <c r="F40">
         <v>200</v>
       </c>
-      <c r="G31">
+      <c r="G40">
         <v>600</v>
       </c>
-      <c r="H31">
+      <c r="H40">
         <v>1400</v>
       </c>
-      <c r="I31">
+      <c r="I40">
         <v>1700</v>
       </c>
-      <c r="J31">
+      <c r="J40">
         <v>2000</v>
       </c>
-      <c r="K31">
+      <c r="K40">
         <v>200</v>
       </c>
-      <c r="L31">
+      <c r="L40">
         <v>200</v>
       </c>
-      <c r="M31">
+      <c r="M40">
         <v>220</v>
       </c>
-      <c r="N31" s="9">
+      <c r="N40" s="9">
         <v>39</v>
       </c>
-      <c r="O31" t="s">
+      <c r="O40" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="P40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A41" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B41" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="E32">
+      <c r="E41">
         <v>-1</v>
       </c>
-      <c r="N32" s="9">
+      <c r="N41" s="11">
         <v>40</v>
       </c>
-      <c r="O32" t="s">
+      <c r="O41" t="s">
         <v>80</v>
       </c>
+      <c r="P41">
+        <v>-1</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N32">
-    <sortCondition ref="N9:N32"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N41">
+    <sortCondition ref="N12:N41"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add code for landing on go
</commit_message>
<xml_diff>
--- a/resources/info.xlsx
+++ b/resources/info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\moi\programming things\0.projects\monopoly-discord-bot\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA62C37-0DD0-43B1-9AFA-A4D1DA4BA72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEC07C5-352D-421A-B7E8-B869E64718EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="89">
   <si>
     <t>PropertyUS</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>Just Visiting Jail</t>
+  </si>
+  <si>
+    <t>START</t>
   </si>
 </sst>
 </file>
@@ -863,7 +866,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -889,7 +892,6 @@
     <xf numFmtId="0" fontId="17" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1254,10 +1256,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P41"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P41" sqref="P41"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1318,333 +1320,297 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N2" s="9">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>60</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="F3">
         <v>10</v>
       </c>
-      <c r="G2">
+      <c r="G3">
         <v>30</v>
       </c>
-      <c r="H2">
+      <c r="H3">
         <v>90</v>
       </c>
-      <c r="I2">
+      <c r="I3">
         <v>160</v>
       </c>
-      <c r="J2">
+      <c r="J3">
         <v>250</v>
       </c>
-      <c r="K2">
+      <c r="K3">
         <v>50</v>
       </c>
-      <c r="L2">
+      <c r="L3">
         <v>30</v>
       </c>
-      <c r="M2">
+      <c r="M3">
         <v>33</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N3" s="11">
         <v>1</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O3" t="s">
         <v>72</v>
       </c>
-      <c r="P2">
+      <c r="P3">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="N3" s="11">
+      <c r="N4" s="11">
         <v>2</v>
       </c>
-      <c r="P3">
+      <c r="P4">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>60</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>4</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>20</v>
       </c>
-      <c r="G4">
+      <c r="G5">
         <v>60</v>
       </c>
-      <c r="H4">
+      <c r="H5">
         <v>180</v>
       </c>
-      <c r="I4">
+      <c r="I5">
         <v>320</v>
       </c>
-      <c r="J4">
+      <c r="J5">
         <v>450</v>
       </c>
-      <c r="K4">
+      <c r="K5">
         <v>50</v>
       </c>
-      <c r="L4">
+      <c r="L5">
         <v>30</v>
       </c>
-      <c r="M4">
+      <c r="M5">
         <v>33</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N5" s="9">
         <v>3</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O5" t="s">
         <v>72</v>
       </c>
-      <c r="P4">
+      <c r="P5">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B6" s="15" t="s">
         <v>69</v>
-      </c>
-      <c r="C5">
-        <v>200</v>
-      </c>
-      <c r="E5">
-        <v>-2</v>
-      </c>
-      <c r="N5" s="9">
-        <v>4</v>
-      </c>
-      <c r="P5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>14</v>
       </c>
       <c r="C6">
         <v>200</v>
       </c>
       <c r="E6">
+        <v>-2</v>
+      </c>
+      <c r="N6" s="9">
+        <v>4</v>
+      </c>
+      <c r="P6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>200</v>
+      </c>
+      <c r="E7">
         <v>8</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>25</v>
       </c>
-      <c r="G6">
+      <c r="G7">
         <v>50</v>
       </c>
-      <c r="H6">
+      <c r="H7">
         <v>100</v>
       </c>
-      <c r="I6">
+      <c r="I7">
         <v>200</v>
       </c>
-      <c r="L6">
+      <c r="L7">
         <v>100</v>
       </c>
-      <c r="M6">
+      <c r="M7">
         <v>110</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N7" s="9">
         <v>5</v>
       </c>
-      <c r="P6">
+      <c r="P7">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>100</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>6</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>1</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>30</v>
       </c>
-      <c r="G7">
+      <c r="G8">
         <v>90</v>
       </c>
-      <c r="H7">
+      <c r="H8">
         <v>270</v>
       </c>
-      <c r="I7">
+      <c r="I8">
         <v>400</v>
       </c>
-      <c r="J7">
+      <c r="J8">
         <v>550</v>
       </c>
-      <c r="K7">
+      <c r="K8">
         <v>50</v>
       </c>
-      <c r="L7">
+      <c r="L8">
         <v>50</v>
       </c>
-      <c r="M7">
+      <c r="M8">
         <v>55</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N8" s="9">
         <v>6</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O8" t="s">
         <v>73</v>
       </c>
-      <c r="P7">
+      <c r="P8">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B9" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="N8" s="11">
+      <c r="N9" s="11">
         <v>7</v>
       </c>
-      <c r="P8">
+      <c r="P9">
         <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9">
-        <v>100</v>
-      </c>
-      <c r="D9">
-        <v>6</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>30</v>
-      </c>
-      <c r="G9">
-        <v>90</v>
-      </c>
-      <c r="H9">
-        <v>270</v>
-      </c>
-      <c r="I9">
-        <v>400</v>
-      </c>
-      <c r="J9">
-        <v>550</v>
-      </c>
-      <c r="K9">
-        <v>50</v>
-      </c>
-      <c r="L9">
-        <v>50</v>
-      </c>
-      <c r="M9">
-        <v>55</v>
-      </c>
-      <c r="N9" s="11">
-        <v>8</v>
-      </c>
-      <c r="O9" t="s">
-        <v>73</v>
-      </c>
-      <c r="P9">
-        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="D10">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G10">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H10">
-        <v>300</v>
+        <v>270</v>
       </c>
       <c r="I10">
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="J10">
-        <v>600</v>
+        <v>550</v>
       </c>
       <c r="K10">
         <v>50</v>
       </c>
       <c r="L10">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="M10">
-        <v>66</v>
-      </c>
-      <c r="N10" s="9">
-        <v>9</v>
+        <v>55</v>
+      </c>
+      <c r="N10" s="11">
+        <v>8</v>
       </c>
       <c r="O10" t="s">
         <v>73</v>
@@ -1654,193 +1620,193 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>120</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>40</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>300</v>
+      </c>
+      <c r="I11">
+        <v>450</v>
+      </c>
+      <c r="J11">
+        <v>600</v>
+      </c>
+      <c r="K11">
+        <v>50</v>
+      </c>
+      <c r="L11">
+        <v>60</v>
+      </c>
+      <c r="M11">
+        <v>66</v>
+      </c>
+      <c r="N11" s="9">
+        <v>9</v>
+      </c>
+      <c r="O11" t="s">
+        <v>73</v>
+      </c>
+      <c r="P11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B12" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="N11" s="9">
+      <c r="N12" s="9">
         <v>10</v>
       </c>
-      <c r="P11">
+      <c r="P12">
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>140</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>10</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>2</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>50</v>
       </c>
-      <c r="G12">
+      <c r="G13">
         <v>150</v>
       </c>
-      <c r="H12">
+      <c r="H13">
         <v>450</v>
       </c>
-      <c r="I12">
+      <c r="I13">
         <v>625</v>
       </c>
-      <c r="J12">
+      <c r="J13">
         <v>750</v>
       </c>
-      <c r="K12">
+      <c r="K13">
         <v>100</v>
       </c>
-      <c r="L12">
+      <c r="L13">
         <v>70</v>
       </c>
-      <c r="M12">
+      <c r="M13">
         <v>77</v>
       </c>
-      <c r="N12" s="9">
+      <c r="N13" s="9">
         <v>11</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O13" t="s">
         <v>74</v>
       </c>
-      <c r="P12">
+      <c r="P13">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13" s="19" t="s">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A14" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B14" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>150</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>9</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <v>4</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>10</v>
       </c>
-      <c r="L13">
+      <c r="L14">
         <v>75</v>
       </c>
-      <c r="M13">
+      <c r="M14">
         <v>83</v>
       </c>
-      <c r="N13" s="9">
+      <c r="N14" s="9">
         <v>12</v>
       </c>
-      <c r="P13">
+      <c r="P14">
         <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14">
-        <v>140</v>
-      </c>
-      <c r="D14">
-        <v>10</v>
-      </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
-      <c r="F14">
-        <v>50</v>
-      </c>
-      <c r="G14">
-        <v>150</v>
-      </c>
-      <c r="H14">
-        <v>450</v>
-      </c>
-      <c r="I14">
-        <v>625</v>
-      </c>
-      <c r="J14">
-        <v>750</v>
-      </c>
-      <c r="K14">
-        <v>100</v>
-      </c>
-      <c r="L14">
-        <v>70</v>
-      </c>
-      <c r="M14">
-        <v>77</v>
-      </c>
-      <c r="N14" s="11">
-        <v>13</v>
-      </c>
-      <c r="O14" t="s">
-        <v>74</v>
-      </c>
-      <c r="P14">
-        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="D15">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
       <c r="F15">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G15">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="H15">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="I15">
-        <v>700</v>
+        <v>625</v>
       </c>
       <c r="J15">
-        <v>900</v>
+        <v>750</v>
       </c>
       <c r="K15">
         <v>100</v>
       </c>
       <c r="L15">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="M15">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="N15" s="11">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O15" t="s">
         <v>74</v>
@@ -1850,199 +1816,199 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>160</v>
+      </c>
+      <c r="D16">
+        <v>12</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>60</v>
+      </c>
+      <c r="G16">
+        <v>180</v>
+      </c>
+      <c r="H16">
+        <v>500</v>
+      </c>
+      <c r="I16">
+        <v>700</v>
+      </c>
+      <c r="J16">
+        <v>900</v>
+      </c>
+      <c r="K16">
+        <v>100</v>
+      </c>
+      <c r="L16">
+        <v>80</v>
+      </c>
+      <c r="M16">
+        <v>88</v>
+      </c>
+      <c r="N16" s="11">
+        <v>14</v>
+      </c>
+      <c r="O16" t="s">
+        <v>74</v>
+      </c>
+      <c r="P16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A17" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B17" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>200</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>8</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <v>25</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>50</v>
       </c>
-      <c r="H16">
+      <c r="H17">
         <v>100</v>
       </c>
-      <c r="I16">
+      <c r="I17">
         <v>200</v>
       </c>
-      <c r="L16">
+      <c r="L17">
         <v>100</v>
       </c>
-      <c r="M16">
+      <c r="M17">
         <v>110</v>
       </c>
-      <c r="N16" s="9">
+      <c r="N17" s="9">
         <v>15</v>
       </c>
-      <c r="P16">
+      <c r="P17">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>180</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>14</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>3</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>70</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>200</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <v>550</v>
       </c>
-      <c r="I17">
+      <c r="I18">
         <v>750</v>
       </c>
-      <c r="J17">
+      <c r="J18">
         <v>950</v>
       </c>
-      <c r="K17">
+      <c r="K18">
         <v>100</v>
       </c>
-      <c r="L17">
+      <c r="L18">
         <v>90</v>
       </c>
-      <c r="M17">
+      <c r="M18">
         <v>99</v>
       </c>
-      <c r="N17" s="9">
+      <c r="N18" s="9">
         <v>16</v>
       </c>
-      <c r="O17" t="s">
+      <c r="O18" t="s">
         <v>75</v>
       </c>
-      <c r="P17">
+      <c r="P18">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A19" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B19" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="N18" s="9">
+      <c r="N19" s="9">
         <v>17</v>
       </c>
-      <c r="P18">
+      <c r="P19">
         <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19">
-        <v>180</v>
-      </c>
-      <c r="D19">
-        <v>14</v>
-      </c>
-      <c r="E19">
-        <v>3</v>
-      </c>
-      <c r="F19">
-        <v>70</v>
-      </c>
-      <c r="G19">
-        <v>200</v>
-      </c>
-      <c r="H19">
-        <v>550</v>
-      </c>
-      <c r="I19">
-        <v>750</v>
-      </c>
-      <c r="J19">
-        <v>950</v>
-      </c>
-      <c r="K19">
-        <v>100</v>
-      </c>
-      <c r="L19">
-        <v>90</v>
-      </c>
-      <c r="M19">
-        <v>99</v>
-      </c>
-      <c r="N19" s="9">
-        <v>18</v>
-      </c>
-      <c r="O19" t="s">
-        <v>75</v>
-      </c>
-      <c r="P19">
-        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C20">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="D20">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E20">
         <v>3</v>
       </c>
       <c r="F20">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="G20">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="H20">
-        <v>600</v>
+        <v>550</v>
       </c>
       <c r="I20">
-        <v>800</v>
+        <v>750</v>
       </c>
       <c r="J20">
-        <v>1000</v>
+        <v>950</v>
       </c>
       <c r="K20">
         <v>100</v>
       </c>
       <c r="L20">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="M20">
-        <v>110</v>
-      </c>
-      <c r="N20" s="11">
-        <v>19</v>
+        <v>99</v>
+      </c>
+      <c r="N20" s="9">
+        <v>18</v>
       </c>
       <c r="O20" t="s">
         <v>75</v>
@@ -2052,175 +2018,175 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21">
+        <v>200</v>
+      </c>
+      <c r="D21">
+        <v>16</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>80</v>
+      </c>
+      <c r="G21">
+        <v>220</v>
+      </c>
+      <c r="H21">
+        <v>600</v>
+      </c>
+      <c r="I21">
+        <v>800</v>
+      </c>
+      <c r="J21">
+        <v>1000</v>
+      </c>
+      <c r="K21">
+        <v>100</v>
+      </c>
+      <c r="L21">
+        <v>100</v>
+      </c>
+      <c r="M21">
+        <v>110</v>
+      </c>
+      <c r="N21" s="11">
+        <v>19</v>
+      </c>
+      <c r="O21" t="s">
+        <v>75</v>
+      </c>
+      <c r="P21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A22" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B22" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="N21" s="11">
+      <c r="N22" s="11">
         <v>20</v>
       </c>
-      <c r="P21">
+      <c r="P22">
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A22" s="4" t="s">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <v>220</v>
       </c>
-      <c r="D22">
+      <c r="D23">
         <v>18</v>
       </c>
-      <c r="E22">
+      <c r="E23">
         <v>4</v>
       </c>
-      <c r="F22">
+      <c r="F23">
         <v>90</v>
       </c>
-      <c r="G22">
+      <c r="G23">
         <v>250</v>
       </c>
-      <c r="H22">
+      <c r="H23">
         <v>700</v>
       </c>
-      <c r="I22">
+      <c r="I23">
         <v>875</v>
       </c>
-      <c r="J22">
+      <c r="J23">
         <v>1050</v>
       </c>
-      <c r="K22">
+      <c r="K23">
         <v>150</v>
       </c>
-      <c r="L22">
+      <c r="L23">
         <v>110</v>
       </c>
-      <c r="M22">
+      <c r="M23">
         <v>121</v>
       </c>
-      <c r="N22" s="9">
+      <c r="N23" s="9">
         <v>21</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O23" t="s">
         <v>76</v>
       </c>
-      <c r="P22">
+      <c r="P23">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="13" t="s">
+    <row r="24" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B24" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="N23" s="11">
+      <c r="N24" s="11">
         <v>22</v>
       </c>
-      <c r="P23">
+      <c r="P24">
         <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24">
-        <v>220</v>
-      </c>
-      <c r="D24">
-        <v>18</v>
-      </c>
-      <c r="E24">
-        <v>4</v>
-      </c>
-      <c r="F24">
-        <v>90</v>
-      </c>
-      <c r="G24">
-        <v>250</v>
-      </c>
-      <c r="H24">
-        <v>700</v>
-      </c>
-      <c r="I24">
-        <v>875</v>
-      </c>
-      <c r="J24">
-        <v>1050</v>
-      </c>
-      <c r="K24">
-        <v>150</v>
-      </c>
-      <c r="L24">
-        <v>110</v>
-      </c>
-      <c r="M24">
-        <v>121</v>
-      </c>
-      <c r="N24" s="11">
-        <v>23</v>
-      </c>
-      <c r="O24" t="s">
-        <v>76</v>
-      </c>
-      <c r="P24">
-        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C25">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="D25">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E25">
         <v>4</v>
       </c>
       <c r="F25">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="G25">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="H25">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="I25">
-        <v>925</v>
+        <v>875</v>
       </c>
       <c r="J25">
-        <v>1100</v>
+        <v>1050</v>
       </c>
       <c r="K25">
         <v>150</v>
       </c>
       <c r="L25">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="M25">
-        <v>132</v>
-      </c>
-      <c r="N25" s="9">
-        <v>24</v>
+        <v>121</v>
+      </c>
+      <c r="N25" s="11">
+        <v>23</v>
       </c>
       <c r="O25" t="s">
         <v>76</v>
@@ -2230,102 +2196,102 @@
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26">
+        <v>240</v>
+      </c>
+      <c r="D26">
+        <v>20</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>100</v>
+      </c>
+      <c r="G26">
+        <v>300</v>
+      </c>
+      <c r="H26">
+        <v>750</v>
+      </c>
+      <c r="I26">
+        <v>925</v>
+      </c>
+      <c r="J26">
+        <v>1100</v>
+      </c>
+      <c r="K26">
+        <v>150</v>
+      </c>
+      <c r="L26">
+        <v>120</v>
+      </c>
+      <c r="M26">
+        <v>132</v>
+      </c>
+      <c r="N26" s="9">
+        <v>24</v>
+      </c>
+      <c r="O26" t="s">
+        <v>76</v>
+      </c>
+      <c r="P26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A27" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B27" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <v>200</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>24</v>
       </c>
-      <c r="E26">
+      <c r="E27">
         <v>8</v>
       </c>
-      <c r="F26">
+      <c r="F27">
         <v>25</v>
       </c>
-      <c r="G26">
+      <c r="G27">
         <v>50</v>
       </c>
-      <c r="H26">
+      <c r="H27">
         <v>100</v>
       </c>
-      <c r="I26">
+      <c r="I27">
         <v>200</v>
       </c>
-      <c r="L26">
+      <c r="L27">
         <v>100</v>
       </c>
-      <c r="M26">
+      <c r="M27">
         <v>110</v>
       </c>
-      <c r="N26" s="9">
+      <c r="N27" s="9">
         <v>25</v>
       </c>
-      <c r="P26">
+      <c r="P27">
         <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A27" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27">
-        <v>260</v>
-      </c>
-      <c r="D27">
-        <v>22</v>
-      </c>
-      <c r="E27">
-        <v>5</v>
-      </c>
-      <c r="F27">
-        <v>110</v>
-      </c>
-      <c r="G27">
-        <v>330</v>
-      </c>
-      <c r="H27">
-        <v>800</v>
-      </c>
-      <c r="I27">
-        <v>975</v>
-      </c>
-      <c r="J27">
-        <v>1150</v>
-      </c>
-      <c r="K27">
-        <v>150</v>
-      </c>
-      <c r="L27">
-        <v>130</v>
-      </c>
-      <c r="M27">
-        <v>143</v>
-      </c>
-      <c r="N27" s="9">
-        <v>26</v>
-      </c>
-      <c r="O27" t="s">
-        <v>77</v>
-      </c>
-      <c r="P27">
-        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C28">
         <v>260</v>
@@ -2361,7 +2327,7 @@
         <v>143</v>
       </c>
       <c r="N28" s="9">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O28" t="s">
         <v>77</v>
@@ -2371,157 +2337,157 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29">
+        <v>260</v>
+      </c>
+      <c r="D29">
+        <v>22</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="F29">
+        <v>110</v>
+      </c>
+      <c r="G29">
+        <v>330</v>
+      </c>
+      <c r="H29">
+        <v>800</v>
+      </c>
+      <c r="I29">
+        <v>975</v>
+      </c>
+      <c r="J29">
+        <v>1150</v>
+      </c>
+      <c r="K29">
+        <v>150</v>
+      </c>
+      <c r="L29">
+        <v>130</v>
+      </c>
+      <c r="M29">
+        <v>143</v>
+      </c>
+      <c r="N29" s="9">
+        <v>27</v>
+      </c>
+      <c r="O29" t="s">
+        <v>77</v>
+      </c>
+      <c r="P29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A30" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B30" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C29">
+      <c r="C30">
         <v>150</v>
       </c>
-      <c r="E29">
+      <c r="E30">
         <v>9</v>
       </c>
-      <c r="F29">
+      <c r="F30">
         <v>4</v>
       </c>
-      <c r="G29">
+      <c r="G30">
         <v>10</v>
       </c>
-      <c r="L29">
+      <c r="L30">
         <v>75</v>
       </c>
-      <c r="M29">
+      <c r="M30">
         <v>83</v>
       </c>
-      <c r="N29" s="11">
+      <c r="N30" s="11">
         <v>28</v>
       </c>
-      <c r="P29">
+      <c r="P30">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A30" s="8" t="s">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A31" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B31" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <v>280</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <v>24</v>
       </c>
-      <c r="E30">
+      <c r="E31">
         <v>5</v>
       </c>
-      <c r="F30">
+      <c r="F31">
         <v>120</v>
       </c>
-      <c r="G30">
+      <c r="G31">
         <v>360</v>
       </c>
-      <c r="H30">
+      <c r="H31">
         <v>850</v>
       </c>
-      <c r="I30">
+      <c r="I31">
         <v>1025</v>
       </c>
-      <c r="J30">
+      <c r="J31">
         <v>1200</v>
       </c>
-      <c r="K30">
+      <c r="K31">
         <v>150</v>
       </c>
-      <c r="L30">
+      <c r="L31">
         <v>140</v>
       </c>
-      <c r="M30">
+      <c r="M31">
         <v>154</v>
       </c>
-      <c r="N30" s="11">
+      <c r="N31" s="11">
         <v>29</v>
       </c>
-      <c r="O30" t="s">
+      <c r="O31" t="s">
         <v>77</v>
       </c>
-      <c r="P30">
+      <c r="P31">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A31" s="20" t="s">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A32" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B32" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="N31" s="9">
+      <c r="N32" s="9">
         <v>30</v>
       </c>
-      <c r="P31">
+      <c r="P32">
         <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32">
-        <v>300</v>
-      </c>
-      <c r="D32">
-        <v>26</v>
-      </c>
-      <c r="E32">
-        <v>6</v>
-      </c>
-      <c r="F32">
-        <v>130</v>
-      </c>
-      <c r="G32">
-        <v>390</v>
-      </c>
-      <c r="H32">
-        <v>900</v>
-      </c>
-      <c r="I32">
-        <v>1100</v>
-      </c>
-      <c r="J32">
-        <v>1275</v>
-      </c>
-      <c r="K32">
-        <v>200</v>
-      </c>
-      <c r="L32">
-        <v>150</v>
-      </c>
-      <c r="M32">
-        <v>165</v>
-      </c>
-      <c r="N32" s="9">
-        <v>31</v>
-      </c>
-      <c r="O32" t="s">
-        <v>78</v>
-      </c>
-      <c r="P32">
-        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C33">
         <v>300</v>
@@ -2557,7 +2523,7 @@
         <v>165</v>
       </c>
       <c r="N33" s="9">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O33" t="s">
         <v>78</v>
@@ -2567,264 +2533,314 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34">
+        <v>300</v>
+      </c>
+      <c r="D34">
+        <v>26</v>
+      </c>
+      <c r="E34">
+        <v>6</v>
+      </c>
+      <c r="F34">
+        <v>130</v>
+      </c>
+      <c r="G34">
+        <v>390</v>
+      </c>
+      <c r="H34">
+        <v>900</v>
+      </c>
+      <c r="I34">
+        <v>1100</v>
+      </c>
+      <c r="J34">
+        <v>1275</v>
+      </c>
+      <c r="K34">
+        <v>200</v>
+      </c>
+      <c r="L34">
+        <v>150</v>
+      </c>
+      <c r="M34">
+        <v>165</v>
+      </c>
+      <c r="N34" s="9">
+        <v>32</v>
+      </c>
+      <c r="O34" t="s">
+        <v>78</v>
+      </c>
+      <c r="P34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A35" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B35" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="N34" s="9">
+      <c r="N35" s="9">
         <v>33</v>
       </c>
-      <c r="P34">
+      <c r="P35">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <v>320</v>
       </c>
-      <c r="D35">
+      <c r="D36">
         <v>28</v>
       </c>
-      <c r="E35">
+      <c r="E36">
         <v>6</v>
       </c>
-      <c r="F35">
+      <c r="F36">
         <v>150</v>
       </c>
-      <c r="G35">
+      <c r="G36">
         <v>450</v>
       </c>
-      <c r="H35">
+      <c r="H36">
         <v>1000</v>
       </c>
-      <c r="I35">
+      <c r="I36">
         <v>1200</v>
       </c>
-      <c r="J35">
+      <c r="J36">
         <v>1400</v>
       </c>
-      <c r="K35">
+      <c r="K36">
         <v>200</v>
       </c>
-      <c r="L35">
+      <c r="L36">
         <v>160</v>
       </c>
-      <c r="M35">
+      <c r="M36">
         <v>176</v>
       </c>
-      <c r="N35" s="11">
+      <c r="N36" s="11">
         <v>34</v>
       </c>
-      <c r="O35" t="s">
+      <c r="O36" t="s">
         <v>78</v>
       </c>
-      <c r="P35">
+      <c r="P36">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A36" s="18" t="s">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A37" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B37" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <v>200</v>
       </c>
-      <c r="E36">
+      <c r="E37">
         <v>8</v>
       </c>
-      <c r="F36">
+      <c r="F37">
         <v>25</v>
       </c>
-      <c r="G36">
+      <c r="G37">
         <v>50</v>
       </c>
-      <c r="H36">
+      <c r="H37">
         <v>100</v>
       </c>
-      <c r="I36">
+      <c r="I37">
         <v>200</v>
       </c>
-      <c r="L36">
+      <c r="L37">
         <v>100</v>
       </c>
-      <c r="M36">
+      <c r="M37">
         <v>110</v>
       </c>
-      <c r="N36" s="11">
+      <c r="N37" s="11">
         <v>35</v>
       </c>
-      <c r="P36">
+      <c r="P37">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A37" s="13" t="s">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A38" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B38" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="N37" s="9">
+      <c r="N38" s="9">
         <v>36</v>
       </c>
-      <c r="P37">
+      <c r="P38">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C38">
+      <c r="C39">
         <v>350</v>
       </c>
-      <c r="D38">
+      <c r="D39">
         <v>35</v>
       </c>
-      <c r="E38">
+      <c r="E39">
         <v>7</v>
       </c>
-      <c r="F38">
+      <c r="F39">
         <v>175</v>
       </c>
-      <c r="G38">
+      <c r="G39">
         <v>500</v>
       </c>
-      <c r="H38">
+      <c r="H39">
         <v>1100</v>
       </c>
-      <c r="I38">
+      <c r="I39">
         <v>1300</v>
       </c>
-      <c r="J38">
+      <c r="J39">
         <v>1500</v>
       </c>
-      <c r="K38">
+      <c r="K39">
         <v>200</v>
       </c>
-      <c r="L38">
+      <c r="L39">
         <v>175</v>
       </c>
-      <c r="M38">
+      <c r="M39">
         <v>193</v>
       </c>
-      <c r="N38" s="9">
+      <c r="N39" s="9">
         <v>37</v>
       </c>
-      <c r="O38" t="s">
+      <c r="O39" t="s">
         <v>79</v>
-      </c>
-      <c r="P38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A39" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C39">
-        <v>100</v>
-      </c>
-      <c r="E39">
-        <v>-2</v>
-      </c>
-      <c r="N39" s="9">
-        <v>38</v>
       </c>
       <c r="P39">
         <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40">
+        <v>100</v>
+      </c>
+      <c r="E40">
+        <v>-2</v>
+      </c>
+      <c r="N40" s="9">
+        <v>38</v>
+      </c>
+      <c r="P40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C40">
+      <c r="C41">
         <v>400</v>
       </c>
-      <c r="D40">
+      <c r="D41">
         <v>50</v>
       </c>
-      <c r="E40">
+      <c r="E41">
         <v>7</v>
       </c>
-      <c r="F40">
+      <c r="F41">
         <v>200</v>
       </c>
-      <c r="G40">
+      <c r="G41">
         <v>600</v>
       </c>
-      <c r="H40">
+      <c r="H41">
         <v>1400</v>
       </c>
-      <c r="I40">
+      <c r="I41">
         <v>1700</v>
       </c>
-      <c r="J40">
+      <c r="J41">
         <v>2000</v>
       </c>
-      <c r="K40">
+      <c r="K41">
         <v>200</v>
       </c>
-      <c r="L40">
+      <c r="L41">
         <v>200</v>
       </c>
-      <c r="M40">
+      <c r="M41">
         <v>220</v>
       </c>
-      <c r="N40" s="9">
+      <c r="N41" s="9">
         <v>39</v>
       </c>
-      <c r="O40" t="s">
+      <c r="O41" t="s">
         <v>79</v>
       </c>
-      <c r="P40">
+      <c r="P41">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A41" s="17" t="s">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A42" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B42" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="E41">
+      <c r="E42">
         <v>-1</v>
       </c>
-      <c r="N41" s="11">
+      <c r="N42" s="11">
         <v>40</v>
       </c>
-      <c r="O41" t="s">
+      <c r="O42" t="s">
         <v>80</v>
       </c>
-      <c r="P41">
+      <c r="P42">
         <v>-1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N41">
-    <sortCondition ref="N12:N41"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:N42">
+    <sortCondition ref="N13:N42"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
moved to directly using xlsx
</commit_message>
<xml_diff>
--- a/resources/info.xlsx
+++ b/resources/info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\moi\programming things\0.projects\monopoly-discord-bot\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEC07C5-352D-421A-B7E8-B869E64718EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D73E35-45FE-4352-ACF6-35D2593F7DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -286,7 +286,7 @@
     <t>Just Visiting Jail</t>
   </si>
   <si>
-    <t>START</t>
+    <t>GO</t>
   </si>
 </sst>
 </file>
@@ -1259,7 +1259,7 @@
   <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
fixed some bugs regarding change to xlsx working on exchange now
</commit_message>
<xml_diff>
--- a/resources/info.xlsx
+++ b/resources/info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\moi\programming things\0.projects\monopoly-discord-bot\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D73E35-45FE-4352-ACF6-35D2593F7DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46AC4E4-CBE1-41CB-B64B-2AEB0F99BD4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="99">
   <si>
     <t>PropertyUS</t>
   </si>
@@ -94,9 +94,6 @@
     <t>Electric Company</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>States Avenue</t>
   </si>
   <si>
@@ -287,6 +284,39 @@
   </si>
   <si>
     <t>GO</t>
+  </si>
+  <si>
+    <t>:triangular_flag_on_post:</t>
+  </si>
+  <si>
+    <t>:game_die:</t>
+  </si>
+  <si>
+    <t>:handbag:</t>
+  </si>
+  <si>
+    <t>:coin:</t>
+  </si>
+  <si>
+    <t>:station:</t>
+  </si>
+  <si>
+    <t>:gem:</t>
+  </si>
+  <si>
+    <t>:police_officer:</t>
+  </si>
+  <si>
+    <t>:police_car:</t>
+  </si>
+  <si>
+    <t>:electric_plug:</t>
+  </si>
+  <si>
+    <t>:blue_car:</t>
+  </si>
+  <si>
+    <t>:potable_water:</t>
   </si>
 </sst>
 </file>
@@ -866,7 +896,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -892,6 +922,9 @@
     <xf numFmtId="0" fontId="17" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1258,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1286,16 +1319,16 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
         <v>64</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>65</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>66</v>
-      </c>
-      <c r="I1" t="s">
-        <v>67</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
@@ -1310,24 +1343,27 @@
         <v>8</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N2" s="9">
         <v>0</v>
+      </c>
+      <c r="O2" t="s">
+        <v>88</v>
       </c>
       <c r="P2">
         <v>7</v>
@@ -1377,7 +1413,7 @@
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P3">
         <v>2</v>
@@ -1385,13 +1421,16 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N4" s="11">
         <v>2</v>
+      </c>
+      <c r="O4" s="21" t="s">
+        <v>90</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -1441,7 +1480,7 @@
         <v>3</v>
       </c>
       <c r="O5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P5">
         <v>2</v>
@@ -1449,10 +1488,10 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6">
         <v>200</v>
@@ -1462,6 +1501,9 @@
       </c>
       <c r="N6" s="9">
         <v>4</v>
+      </c>
+      <c r="O6" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="P6">
         <v>4</v>
@@ -1501,6 +1543,9 @@
       <c r="N7" s="9">
         <v>5</v>
       </c>
+      <c r="O7" s="21" t="s">
+        <v>92</v>
+      </c>
       <c r="P7">
         <v>5</v>
       </c>
@@ -1549,7 +1594,7 @@
         <v>6</v>
       </c>
       <c r="O8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P8">
         <v>2</v>
@@ -1557,13 +1602,16 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N9" s="11">
         <v>7</v>
+      </c>
+      <c r="O9" s="21" t="s">
+        <v>89</v>
       </c>
       <c r="P9">
         <v>1</v>
@@ -1613,7 +1661,7 @@
         <v>8</v>
       </c>
       <c r="O10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P10">
         <v>2</v>
@@ -1663,7 +1711,7 @@
         <v>9</v>
       </c>
       <c r="O11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P11">
         <v>2</v>
@@ -1671,13 +1719,16 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N12" s="9">
         <v>10</v>
+      </c>
+      <c r="O12" s="21" t="s">
+        <v>94</v>
       </c>
       <c r="P12">
         <v>-1</v>
@@ -1727,7 +1778,7 @@
         <v>11</v>
       </c>
       <c r="O13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P13">
         <v>2</v>
@@ -1761,16 +1812,19 @@
       <c r="N14" s="9">
         <v>12</v>
       </c>
+      <c r="O14" s="21" t="s">
+        <v>96</v>
+      </c>
       <c r="P14">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="C15">
         <v>140</v>
@@ -1809,7 +1863,7 @@
         <v>13</v>
       </c>
       <c r="O15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P15">
         <v>2</v>
@@ -1817,10 +1871,10 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="C16">
         <v>160</v>
@@ -1859,7 +1913,7 @@
         <v>14</v>
       </c>
       <c r="O16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P16">
         <v>2</v>
@@ -1867,10 +1921,10 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17">
         <v>200</v>
@@ -1899,16 +1953,19 @@
       <c r="N17" s="9">
         <v>15</v>
       </c>
+      <c r="O17" s="21" t="s">
+        <v>92</v>
+      </c>
       <c r="P17">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="C18">
         <v>180</v>
@@ -1947,7 +2004,7 @@
         <v>16</v>
       </c>
       <c r="O18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P18">
         <v>2</v>
@@ -1955,24 +2012,27 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N19" s="9">
         <v>17</v>
       </c>
+      <c r="O19" s="21" t="s">
+        <v>90</v>
+      </c>
       <c r="P19">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="C20">
         <v>180</v>
@@ -2011,7 +2071,7 @@
         <v>18</v>
       </c>
       <c r="O20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P20">
         <v>2</v>
@@ -2019,10 +2079,10 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="C21">
         <v>200</v>
@@ -2061,7 +2121,7 @@
         <v>19</v>
       </c>
       <c r="O21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P21">
         <v>2</v>
@@ -2069,24 +2129,27 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N22" s="11">
         <v>20</v>
       </c>
+      <c r="O22" s="21" t="s">
+        <v>97</v>
+      </c>
       <c r="P22">
         <v>-1</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="C23">
         <v>220</v>
@@ -2125,7 +2188,7 @@
         <v>21</v>
       </c>
       <c r="O23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P23">
         <v>2</v>
@@ -2133,24 +2196,27 @@
     </row>
     <row r="24" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N24" s="11">
         <v>22</v>
       </c>
+      <c r="O24" s="21" t="s">
+        <v>89</v>
+      </c>
       <c r="P24">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="C25">
         <v>220</v>
@@ -2189,7 +2255,7 @@
         <v>23</v>
       </c>
       <c r="O25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P25">
         <v>2</v>
@@ -2197,10 +2263,10 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="C26">
         <v>240</v>
@@ -2239,7 +2305,7 @@
         <v>24</v>
       </c>
       <c r="O26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P26">
         <v>2</v>
@@ -2247,17 +2313,14 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C27">
         <v>200</v>
       </c>
-      <c r="D27" t="s">
-        <v>24</v>
-      </c>
       <c r="E27">
         <v>8</v>
       </c>
@@ -2282,16 +2345,19 @@
       <c r="N27" s="9">
         <v>25</v>
       </c>
+      <c r="O27" s="21" t="s">
+        <v>92</v>
+      </c>
       <c r="P27">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>44</v>
       </c>
       <c r="C28">
         <v>260</v>
@@ -2330,7 +2396,7 @@
         <v>26</v>
       </c>
       <c r="O28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P28">
         <v>2</v>
@@ -2338,10 +2404,10 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>46</v>
       </c>
       <c r="C29">
         <v>260</v>
@@ -2380,7 +2446,7 @@
         <v>27</v>
       </c>
       <c r="O29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P29">
         <v>2</v>
@@ -2388,10 +2454,10 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C30">
         <v>150</v>
@@ -2414,16 +2480,19 @@
       <c r="N30" s="11">
         <v>28</v>
       </c>
+      <c r="O30" s="21" t="s">
+        <v>98</v>
+      </c>
       <c r="P30">
         <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="C31">
         <v>280</v>
@@ -2462,7 +2531,7 @@
         <v>29</v>
       </c>
       <c r="O31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P31">
         <v>2</v>
@@ -2470,24 +2539,27 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N32" s="9">
         <v>30</v>
       </c>
+      <c r="O32" s="21" t="s">
+        <v>95</v>
+      </c>
       <c r="P32">
         <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="C33">
         <v>300</v>
@@ -2526,7 +2598,7 @@
         <v>31</v>
       </c>
       <c r="O33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P33">
         <v>2</v>
@@ -2534,10 +2606,10 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="C34">
         <v>300</v>
@@ -2576,7 +2648,7 @@
         <v>32</v>
       </c>
       <c r="O34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P34">
         <v>2</v>
@@ -2584,24 +2656,27 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N35" s="9">
         <v>33</v>
       </c>
+      <c r="O35" s="21" t="s">
+        <v>90</v>
+      </c>
       <c r="P35">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="C36">
         <v>320</v>
@@ -2640,7 +2715,7 @@
         <v>34</v>
       </c>
       <c r="O36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P36">
         <v>2</v>
@@ -2648,10 +2723,10 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="18" t="s">
         <v>56</v>
-      </c>
-      <c r="B37" s="18" t="s">
-        <v>57</v>
       </c>
       <c r="C37">
         <v>200</v>
@@ -2680,30 +2755,36 @@
       <c r="N37" s="11">
         <v>35</v>
       </c>
+      <c r="O37" s="21" t="s">
+        <v>92</v>
+      </c>
       <c r="P37">
         <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N38" s="9">
         <v>36</v>
       </c>
+      <c r="O38" s="21" t="s">
+        <v>89</v>
+      </c>
       <c r="P38">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="C39">
         <v>350</v>
@@ -2742,7 +2823,7 @@
         <v>37</v>
       </c>
       <c r="O39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P39">
         <v>2</v>
@@ -2750,10 +2831,10 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C40">
         <v>100</v>
@@ -2764,16 +2845,19 @@
       <c r="N40" s="9">
         <v>38</v>
       </c>
+      <c r="O40" s="21" t="s">
+        <v>93</v>
+      </c>
       <c r="P40">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="C41">
         <v>400</v>
@@ -2812,7 +2896,7 @@
         <v>39</v>
       </c>
       <c r="O41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P41">
         <v>4</v>
@@ -2820,10 +2904,10 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E42">
         <v>-1</v>
@@ -2832,7 +2916,7 @@
         <v>40</v>
       </c>
       <c r="O42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P42">
         <v>-1</v>

</xml_diff>

<commit_message>
added mapmovement for stations and companies
</commit_message>
<xml_diff>
--- a/resources/info.xlsx
+++ b/resources/info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\moi\programming things\0.projects\monopoly-discord-bot\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7563703F-70DA-487F-B5C4-1162757668F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3BF14B-3B27-4D92-BB84-43580482A5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1291,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P42" sqref="P42"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1519,6 +1519,9 @@
       <c r="C7">
         <v>200</v>
       </c>
+      <c r="D7">
+        <v>25</v>
+      </c>
       <c r="E7">
         <v>8</v>
       </c>
@@ -1929,6 +1932,9 @@
       <c r="C17">
         <v>200</v>
       </c>
+      <c r="D17">
+        <v>25</v>
+      </c>
       <c r="E17">
         <v>8</v>
       </c>
@@ -2321,6 +2327,9 @@
       <c r="C27">
         <v>200</v>
       </c>
+      <c r="D27">
+        <v>25</v>
+      </c>
       <c r="E27">
         <v>8</v>
       </c>
@@ -2730,6 +2739,9 @@
       </c>
       <c r="C37">
         <v>200</v>
+      </c>
+      <c r="D37">
+        <v>25</v>
       </c>
       <c r="E37">
         <v>8</v>

</xml_diff>